<commit_message>
update testcase login and DocGiaGUI
</commit_message>
<xml_diff>
--- a/test-case-example.xlsx
+++ b/test-case-example.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Học tập\Kiểm thử phần mềm\BTlon\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Khoa Pham\Documents\kiemthu\QuanLyThuVien\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{918C83EF-5FDE-4D3B-9364-E0673D4DAC1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{618E6794-CC06-4056-87F5-B7A61AC58F6B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="821" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="821" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="97" r:id="rId1"/>
@@ -30,80 +30,14 @@
     <definedName name="Port">[1]Validation!$F$2:$F$40</definedName>
     <definedName name="VancoProducts">[1]Validation!$B$2:$B$4</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="181029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="145">
   <si>
     <t>31/07/2007</t>
-  </si>
-  <si>
-    <r>
-      <t>Don't see</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> a new selector: "</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-      </rPr>
-      <t>Export all Carriers"</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>See</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> a new selector: "</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-      </rPr>
-      <t>Export all Carriers"</t>
-    </r>
-  </si>
-  <si>
-    <t>TC1</t>
-  </si>
-  <si>
-    <t>TC2</t>
-  </si>
-  <si>
-    <t>TC3</t>
   </si>
   <si>
     <t>Fail</t>
@@ -248,42 +182,9 @@
     <t>1.0</t>
   </si>
   <si>
-    <t>Checking new role is added</t>
-  </si>
-  <si>
     <t>CR236 "Export all carrier choices"</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Checking new function is added in </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-      </rPr>
-      <t>Classic or Current Mode</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Role Tab is added a new role, it's name "</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-      </rPr>
-      <t>CanExportAllCarrierChoices"</t>
-    </r>
-  </si>
-  <si>
     <t>Check set Role CanExportAllCarrierChoices = False</t>
   </si>
   <si>
@@ -314,32 +215,348 @@
     <t xml:space="preserve">CR1 - </t>
   </si>
   <si>
-    <t xml:space="preserve">1: Go to the system TestProEngine with Classic or Current or Expert Mode
-2: Go to maintenance 
-3: Click Maintenance Users
-4: Click Role Tab
+    <t>John Doe</t>
+  </si>
+  <si>
+    <t>Jane Doe</t>
+  </si>
+  <si>
+    <t>1.Kiểm tra form Login</t>
+  </si>
+  <si>
+    <t>LG1</t>
+  </si>
+  <si>
+    <t>Kiểm tra đăng nhập chỉ nhập username mà không nhập password</t>
+  </si>
+  <si>
+    <t>Hiện thanh thông báo :" Please enter your name and pasword"</t>
+  </si>
+  <si>
+    <t>LG2</t>
+  </si>
+  <si>
+    <t>kiểm tra đăng nhập không nhập username và chỉ nhập password</t>
+  </si>
+  <si>
+    <t>LG3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1: Nhập chính xác username
+2: Nhập chính xác password 
+3: Click vào nút DocGiaLogin
 </t>
   </si>
   <si>
-    <t>1: Go to the system TestProEngine with Classic or Current  Mode that has to set role "CanExportAllCarrierChoices"
-2: Submit for the quote 
-3: Open the quote at the home
-4: Go to Quick Links</t>
-  </si>
-  <si>
-    <t>1: Go to the system TestProEngine with Classic or Current  Mode that has not to set role "CanExportAllCarrierChoices"
-2: Submit for the quote 
-3: Open the quote at the home
-4: Go to Quick Links</t>
-  </si>
-  <si>
-    <t>John Doe</t>
-  </si>
-  <si>
-    <t>Jane Doe</t>
-  </si>
-  <si>
-    <t>1.Kiểm tra form Login</t>
+    <t>LG4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kiểm tra đăng nhập mà không nhập username và password </t>
+  </si>
+  <si>
+    <t>1: Click vào nút DocGiaLogin</t>
+  </si>
+  <si>
+    <t>LG5</t>
+  </si>
+  <si>
+    <t>Kiểm tra đăng nhập nhập sai username và nhập đúng password</t>
+  </si>
+  <si>
+    <t>Kiểm tra đăng nhập nhập đúng username và nhập sai password</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1: Nhập đúng username
+2: Nhập sai password 
+3: Click vào nút DocGiaLogin
+</t>
+  </si>
+  <si>
+    <t>Hiện thanh thông báo:" login failed: Wrong username or password"</t>
+  </si>
+  <si>
+    <t>Kiểm tra đăng nhập nhập sai username và nhập sai password</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1: Nhập sai username
+2: Nhập đúng password 
+3: Click vào nút DocGiaLogin
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1: Nhập sai username
+2: Nhập sai password 
+3: Click vào nút DocGiaLogin
+</t>
+  </si>
+  <si>
+    <t>LG6</t>
+  </si>
+  <si>
+    <t>LG7</t>
+  </si>
+  <si>
+    <t>Hiện thanh thông báo :"Login success" và nút Ok</t>
+  </si>
+  <si>
+    <t>Kiểm tra đăng nhập nhập đầy đủ chính xác username và password của tài khoản độc giả</t>
+  </si>
+  <si>
+    <t>Kiểm tra đăng nhập nhập đầy đủ chính xác username và password của tài khoản Nhân viên</t>
+  </si>
+  <si>
+    <t>LG8</t>
+  </si>
+  <si>
+    <t>LG9</t>
+  </si>
+  <si>
+    <t>Kiểm tra nút ok tại thanh thông báo :"Login success"</t>
+  </si>
+  <si>
+    <t>1: Nhập đúng username
+2: Nhập đúng password 
+3: Click vào nút DocGiaLogin
+4: Click vào nút Ok</t>
+  </si>
+  <si>
+    <t>Hiện ra giao diện DocGiaGUI</t>
+  </si>
+  <si>
+    <t>LG10</t>
+  </si>
+  <si>
+    <t>Kiểm tra cho phép copy paste chính xác username và password</t>
+  </si>
+  <si>
+    <t>Kiểm tra copy paste sai username và password</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1: Nhập password
+2: Click vào nút DocGiaLogin
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1: Nhập username 
+2: Click vào nút DocGiaLogin 
+</t>
+  </si>
+  <si>
+    <t>1: Copy và paste sai username
+2: Copy và paste sai password
+3: Click vào nút DocGiaLogin</t>
+  </si>
+  <si>
+    <t>Kiểm tra copy paste sai username và đúng password</t>
+  </si>
+  <si>
+    <t>1: Copy và paste sai username
+2: Copy và paste đúng password
+3: Click vào nút DocGiaLogin</t>
+  </si>
+  <si>
+    <t>Kiểm tra copy paste đúng username và sai password</t>
+  </si>
+  <si>
+    <t>1: Copy và paste đúng username
+2: Copy và paste sai password
+3: Click vào nút DocGiaLogin</t>
+  </si>
+  <si>
+    <t>Kiểm tra độ dài kí tự được phép nhập vào username và password</t>
+  </si>
+  <si>
+    <t>1: Nhập quá 200 kí tự vào username
+2: nhập quá 100 kí tự vào password
+3: Click vào nút DocGiaLogin</t>
+  </si>
+  <si>
+    <t>Hiện thanh thông báo không cho phép nhập quá 50 kí tự</t>
+  </si>
+  <si>
+    <t>LG11</t>
+  </si>
+  <si>
+    <t>LG12</t>
+  </si>
+  <si>
+    <t>LG13</t>
+  </si>
+  <si>
+    <t>LG14</t>
+  </si>
+  <si>
+    <t>1.2 kiểm tra đăng nhập với nút NhanVienLogin</t>
+  </si>
+  <si>
+    <t>1.1 kiểm tra đăng nhập với nút DocGiaLogin</t>
+  </si>
+  <si>
+    <t>LG01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1: Nhập username 
+2: Click vào nút NhanVienLogin 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1: Nhập password
+2: Click vào nút NhanVienLogin 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1: Nhập chính xác username
+2: Nhập chính xác password 
+3: Click vào nút NhanVienLogin
+</t>
+  </si>
+  <si>
+    <t>Hiện thông báo không có quyền truy cập</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1: Click vào nút NhanVienLogin
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1: Nhập sai username
+2: Nhập đúng password 
+3: Click vào nút NhanVienLogin
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1: Nhập đúng username
+2: Nhập sai password 
+3: Click vào nút NhanVienLogin
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1: Nhập sai username
+2: Nhập sai password 
+3: Click vào nút NhanVienLogin
+</t>
+  </si>
+  <si>
+    <t>pass</t>
+  </si>
+  <si>
+    <t>1: Nhập đúng username
+2: Nhập đúng password 
+3: Click vào nút NhanVienLogin
+4: Click vào nút Ok</t>
+  </si>
+  <si>
+    <t>1: Copy và paste chính xác username 
+2: Copy và paste chính xác password 
+3: Click vào nút DocGiaLogin</t>
+  </si>
+  <si>
+    <t>1: Copy và paste chính xác username 
+2: Copy và paste chính xác password 
+3: Click vào nút NhanVienLogin</t>
+  </si>
+  <si>
+    <t>1: Copy và paste sai username
+2: Copy và paste sai password
+3: Click vào nút NhanVienLogin</t>
+  </si>
+  <si>
+    <t>1: Copy và paste sai username
+2: Copy và paste đúng password
+3: Click vào nút NhanVienLogin</t>
+  </si>
+  <si>
+    <t>1: Copy và paste đúng username
+2: Copy và paste sai password
+3: Click vào nút NhanVienLogin</t>
+  </si>
+  <si>
+    <t>1: Nhập quá 200 kí tự vào username
+2: nhập quá 100 kí tự vào password
+3: Click vào nút NhanVienLogin</t>
+  </si>
+  <si>
+    <t>LG014</t>
+  </si>
+  <si>
+    <t>LG013</t>
+  </si>
+  <si>
+    <t>LG012</t>
+  </si>
+  <si>
+    <t>LG011</t>
+  </si>
+  <si>
+    <t>LG010</t>
+  </si>
+  <si>
+    <t>LG09</t>
+  </si>
+  <si>
+    <t>LG08</t>
+  </si>
+  <si>
+    <t>LG07</t>
+  </si>
+  <si>
+    <t>LG06</t>
+  </si>
+  <si>
+    <t>LG05</t>
+  </si>
+  <si>
+    <t>LG04</t>
+  </si>
+  <si>
+    <t>LG03</t>
+  </si>
+  <si>
+    <t>LG02</t>
+  </si>
+  <si>
+    <t>2.Kiểm tra form DocGiaGUI</t>
+  </si>
+  <si>
+    <t>DG1</t>
+  </si>
+  <si>
+    <t>Kiểm tra nút Xem thông tin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1: Click vào nút Xem thông tin 
+</t>
+  </si>
+  <si>
+    <t>DG2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1: Click vào nút Tra cứu sách 
+</t>
+  </si>
+  <si>
+    <t>Kiểm tra nút Log out</t>
+  </si>
+  <si>
+    <t>Kiểm tra nút Tra cứu sách</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1: Click vào nút Log out
+</t>
+  </si>
+  <si>
+    <t>DG3</t>
+  </si>
+  <si>
+    <t>Đăng xuất tài khoản và trở về giao diện login</t>
+  </si>
+  <si>
+    <t>Hiện ra giao diện Thedocgia</t>
+  </si>
+  <si>
+    <t>Hiện ra giao diện Tracuusach</t>
+  </si>
+  <si>
+    <t>Hiện ra giao diện NhanVienGUI</t>
   </si>
 </sst>
 </file>
@@ -999,7 +1216,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="146">
+  <cellXfs count="147">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -1266,33 +1483,96 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="22" fillId="4" borderId="22" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="4" borderId="17" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="23" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="24" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="20" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="22" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="25" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="20" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="22" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="17" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="20" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="22" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="25" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="26" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="27" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="30" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="30" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="22" fillId="4" borderId="20" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="4" borderId="22" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1302,69 +1582,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="20" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="22" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="25" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="20" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="22" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="17" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="20" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="22" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="25" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="26" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="27" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="30" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="30" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="5" borderId="31" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1379,6 +1596,9 @@
     </xf>
     <xf numFmtId="0" fontId="15" fillId="5" borderId="34" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="20" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1740,16 +1960,16 @@
       <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="9" style="1"/>
-    <col min="2" max="2" width="14.109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="14.125" style="1" customWidth="1"/>
     <col min="3" max="3" width="9" style="1"/>
     <col min="4" max="4" width="15" style="1" customWidth="1"/>
-    <col min="5" max="5" width="32.44140625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="23.77734375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="20.44140625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="26.6640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="32.5" style="1" customWidth="1"/>
+    <col min="6" max="6" width="23.75" style="1" customWidth="1"/>
+    <col min="7" max="7" width="20.5" style="1" customWidth="1"/>
+    <col min="8" max="8" width="26.625" style="1" customWidth="1"/>
     <col min="9" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
@@ -1757,10 +1977,10 @@
       <c r="B1" s="31"/>
       <c r="C1" s="31"/>
     </row>
-    <row r="2" spans="1:8" ht="22.2">
+    <row r="2" spans="1:8" ht="22.5">
       <c r="A2" s="26"/>
       <c r="B2" s="27" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C2" s="26"/>
       <c r="D2" s="26"/>
@@ -1771,7 +1991,7 @@
     <row r="3" spans="1:8">
       <c r="A3" s="26"/>
       <c r="B3" s="28" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C3" s="63">
         <v>1.2</v>
@@ -1784,7 +2004,7 @@
     <row r="4" spans="1:8">
       <c r="A4" s="26"/>
       <c r="B4" s="28" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C4" s="11" t="s">
         <v>0</v>
@@ -1794,7 +2014,7 @@
       <c r="F4" s="26"/>
       <c r="G4" s="26"/>
     </row>
-    <row r="5" spans="1:8" ht="14.4" thickBot="1">
+    <row r="5" spans="1:8" ht="15" thickBot="1">
       <c r="A5" s="26"/>
       <c r="B5" s="28"/>
       <c r="C5" s="29"/>
@@ -1806,26 +2026,26 @@
     <row r="6" spans="1:8" ht="14.25" customHeight="1" thickBot="1">
       <c r="A6" s="26"/>
       <c r="B6" s="28" t="s">
-        <v>38</v>
-      </c>
-      <c r="C6" s="111" t="s">
-        <v>53</v>
-      </c>
-      <c r="D6" s="111"/>
-      <c r="E6" s="112"/>
+        <v>33</v>
+      </c>
+      <c r="C6" s="112" t="s">
+        <v>45</v>
+      </c>
+      <c r="D6" s="112"/>
+      <c r="E6" s="113"/>
       <c r="F6" s="26"/>
       <c r="G6" s="26"/>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="26"/>
       <c r="B7" s="28" t="s">
-        <v>39</v>
-      </c>
-      <c r="C7" s="111" t="s">
-        <v>54</v>
-      </c>
-      <c r="D7" s="111"/>
-      <c r="E7" s="112"/>
+        <v>34</v>
+      </c>
+      <c r="C7" s="112" t="s">
+        <v>46</v>
+      </c>
+      <c r="D7" s="112"/>
+      <c r="E7" s="113"/>
       <c r="F7" s="26"/>
       <c r="G7" s="26"/>
     </row>
@@ -1849,94 +2069,94 @@
     </row>
     <row r="10" spans="1:8">
       <c r="B10" s="5" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" s="36" customFormat="1" ht="26.4">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" s="36" customFormat="1" ht="25.5">
       <c r="B11" s="52" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C11" s="53" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="D11" s="53" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="E11" s="53" t="s">
+        <v>7</v>
+      </c>
+      <c r="F11" s="53" t="s">
+        <v>13</v>
+      </c>
+      <c r="G11" s="54" t="s">
         <v>12</v>
       </c>
-      <c r="F11" s="53" t="s">
-        <v>18</v>
-      </c>
-      <c r="G11" s="54" t="s">
-        <v>17</v>
-      </c>
       <c r="H11" s="90" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" s="36" customFormat="1" ht="26.4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" s="36" customFormat="1">
       <c r="B12" s="38">
         <v>39293</v>
       </c>
       <c r="C12" s="39" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="D12" s="40"/>
       <c r="E12" s="41" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="F12" s="77" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="G12" s="89"/>
       <c r="H12" s="91" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" s="36" customFormat="1" ht="26.4">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" s="36" customFormat="1">
       <c r="B13" s="103">
         <v>39295</v>
       </c>
       <c r="C13" s="39" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="D13" s="40"/>
       <c r="E13" s="41" t="s">
+        <v>43</v>
+      </c>
+      <c r="F13" s="77" t="s">
         <v>51</v>
       </c>
-      <c r="F13" s="77" t="s">
-        <v>62</v>
-      </c>
       <c r="G13" s="102" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="H13" s="91" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" s="37" customFormat="1" ht="26.4">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" s="37" customFormat="1" ht="12.75">
       <c r="B14" s="38">
         <v>39311</v>
       </c>
       <c r="C14" s="39" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="D14" s="40"/>
       <c r="E14" s="41" t="s">
+        <v>43</v>
+      </c>
+      <c r="F14" s="77" t="s">
         <v>51</v>
       </c>
-      <c r="F14" s="77" t="s">
-        <v>62</v>
-      </c>
       <c r="G14" s="102" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="H14" s="91" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" s="37" customFormat="1" ht="13.2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" s="37" customFormat="1" ht="12.75">
       <c r="B15" s="45"/>
       <c r="C15" s="46"/>
       <c r="D15" s="43"/>
@@ -2036,31 +2256,31 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:K53"/>
+  <dimension ref="A1:K80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="H47" sqref="H47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8" outlineLevelRow="1"/>
+  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="14.25" outlineLevelRow="1"/>
   <cols>
-    <col min="1" max="1" width="15.6640625" customWidth="1"/>
-    <col min="2" max="2" width="18.109375" style="95" customWidth="1"/>
-    <col min="3" max="3" width="42.109375" customWidth="1"/>
-    <col min="6" max="6" width="23.6640625" customWidth="1"/>
-    <col min="7" max="7" width="18.44140625" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="17.109375" customWidth="1"/>
+    <col min="1" max="1" width="15.625" customWidth="1"/>
+    <col min="2" max="2" width="18.125" style="95" customWidth="1"/>
+    <col min="3" max="3" width="42.125" customWidth="1"/>
+    <col min="6" max="6" width="23.625" customWidth="1"/>
+    <col min="7" max="7" width="18.5" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="17.125" customWidth="1"/>
     <col min="9" max="9" width="9" style="98"/>
     <col min="10" max="10" width="18" style="97" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="2" customFormat="1" ht="12.75" customHeight="1">
       <c r="A1" s="64" t="s">
-        <v>8</v>
-      </c>
-      <c r="B1" s="120"/>
-      <c r="C1" s="120"/>
-      <c r="D1" s="120"/>
+        <v>3</v>
+      </c>
+      <c r="B1" s="114"/>
+      <c r="C1" s="114"/>
+      <c r="D1" s="114"/>
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
       <c r="G1" s="6"/>
@@ -2071,9 +2291,9 @@
     </row>
     <row r="2" spans="1:11" s="2" customFormat="1" ht="11.25" customHeight="1" thickBot="1">
       <c r="A2" s="7"/>
-      <c r="B2" s="121"/>
-      <c r="C2" s="121"/>
-      <c r="D2" s="121"/>
+      <c r="B2" s="115"/>
+      <c r="C2" s="115"/>
+      <c r="D2" s="115"/>
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
@@ -2084,106 +2304,106 @@
     </row>
     <row r="3" spans="1:11" s="3" customFormat="1" ht="15" customHeight="1">
       <c r="A3" s="65" t="s">
-        <v>40</v>
-      </c>
-      <c r="B3" s="111" t="s">
-        <v>56</v>
-      </c>
-      <c r="C3" s="111"/>
-      <c r="D3" s="112"/>
+        <v>35</v>
+      </c>
+      <c r="B3" s="112" t="s">
+        <v>48</v>
+      </c>
+      <c r="C3" s="112"/>
+      <c r="D3" s="113"/>
       <c r="E3" s="68"/>
       <c r="F3" s="68"/>
       <c r="G3" s="68"/>
-      <c r="H3" s="130"/>
-      <c r="I3" s="130"/>
-      <c r="J3" s="130"/>
+      <c r="H3" s="124"/>
+      <c r="I3" s="124"/>
+      <c r="J3" s="124"/>
       <c r="K3" s="9"/>
     </row>
-    <row r="4" spans="1:11" s="3" customFormat="1" ht="13.2">
+    <row r="4" spans="1:11" s="3" customFormat="1" ht="12.75">
       <c r="A4" s="72" t="s">
-        <v>41</v>
-      </c>
-      <c r="B4" s="131" t="s">
-        <v>57</v>
-      </c>
-      <c r="C4" s="132"/>
-      <c r="D4" s="133"/>
+        <v>36</v>
+      </c>
+      <c r="B4" s="126" t="s">
+        <v>49</v>
+      </c>
+      <c r="C4" s="127"/>
+      <c r="D4" s="128"/>
       <c r="E4" s="68"/>
       <c r="F4" s="68"/>
       <c r="G4" s="68"/>
-      <c r="H4" s="130"/>
-      <c r="I4" s="130"/>
-      <c r="J4" s="130"/>
+      <c r="H4" s="124"/>
+      <c r="I4" s="124"/>
+      <c r="J4" s="124"/>
       <c r="K4" s="9"/>
     </row>
-    <row r="5" spans="1:11" s="81" customFormat="1" ht="26.4">
+    <row r="5" spans="1:11" s="81" customFormat="1" ht="12.75">
       <c r="A5" s="72" t="s">
-        <v>34</v>
-      </c>
-      <c r="B5" s="123" t="s">
-        <v>58</v>
-      </c>
-      <c r="C5" s="124"/>
-      <c r="D5" s="125"/>
+        <v>29</v>
+      </c>
+      <c r="B5" s="117" t="s">
+        <v>50</v>
+      </c>
+      <c r="C5" s="118"/>
+      <c r="D5" s="119"/>
       <c r="E5" s="79"/>
       <c r="F5" s="79"/>
       <c r="G5" s="79"/>
-      <c r="H5" s="129"/>
-      <c r="I5" s="129"/>
-      <c r="J5" s="129"/>
+      <c r="H5" s="123"/>
+      <c r="I5" s="123"/>
+      <c r="J5" s="123"/>
       <c r="K5" s="80"/>
     </row>
     <row r="6" spans="1:11" s="3" customFormat="1" ht="15" customHeight="1">
       <c r="A6" s="12" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B6" s="92">
-        <f>COUNTIF(I12:I16,"Pass")</f>
-        <v>4</v>
+        <f>COUNTIF(I12:I18,"Pass")</f>
+        <v>5</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="D6" s="13">
-        <f>COUNTIF(I10:I734,"Pending")</f>
+        <f>COUNTIF(I10:I763,"Pending")</f>
         <v>0</v>
       </c>
       <c r="E6" s="8"/>
       <c r="F6" s="8"/>
       <c r="G6" s="8"/>
-      <c r="H6" s="130"/>
-      <c r="I6" s="130"/>
-      <c r="J6" s="130"/>
+      <c r="H6" s="124"/>
+      <c r="I6" s="124"/>
+      <c r="J6" s="124"/>
       <c r="K6" s="9"/>
     </row>
     <row r="7" spans="1:11" s="3" customFormat="1" ht="15" customHeight="1" thickBot="1">
       <c r="A7" s="14" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B7" s="93">
-        <f>COUNTIF(I12:I17,"Fail")</f>
+        <f>COUNTIF(I12:I27,"Fail")</f>
         <v>1</v>
       </c>
       <c r="C7" s="30" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="D7" s="66">
-        <f>COUNTA(A12:A17)-3</f>
-        <v>3</v>
+        <f>COUNTA(A12:A27)-3</f>
+        <v>13</v>
       </c>
       <c r="E7" s="69"/>
       <c r="F7" s="69"/>
       <c r="G7" s="69"/>
-      <c r="H7" s="130"/>
-      <c r="I7" s="130"/>
-      <c r="J7" s="130"/>
+      <c r="H7" s="124"/>
+      <c r="I7" s="124"/>
+      <c r="J7" s="124"/>
       <c r="K7" s="9"/>
     </row>
     <row r="8" spans="1:11" s="3" customFormat="1" ht="15" customHeight="1">
-      <c r="A8" s="122"/>
-      <c r="B8" s="122"/>
-      <c r="C8" s="122"/>
-      <c r="D8" s="122"/>
+      <c r="A8" s="116"/>
+      <c r="B8" s="116"/>
+      <c r="C8" s="116"/>
+      <c r="D8" s="116"/>
       <c r="E8" s="8"/>
       <c r="F8" s="8"/>
       <c r="G8" s="8"/>
@@ -2193,232 +2413,880 @@
       <c r="K8" s="9"/>
     </row>
     <row r="9" spans="1:11" s="83" customFormat="1" ht="12" customHeight="1">
-      <c r="A9" s="138" t="s">
-        <v>35</v>
-      </c>
-      <c r="B9" s="139" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" s="138" t="s">
-        <v>20</v>
+      <c r="A9" s="133" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9" s="134" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="133" t="s">
+        <v>15</v>
       </c>
       <c r="D9" s="141" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="E9" s="142"/>
       <c r="F9" s="142"/>
       <c r="G9" s="143"/>
-      <c r="H9" s="134" t="s">
+      <c r="H9" s="129" t="s">
+        <v>26</v>
+      </c>
+      <c r="I9" s="125" t="s">
+        <v>5</v>
+      </c>
+      <c r="J9" s="125" t="s">
         <v>31</v>
       </c>
-      <c r="I9" s="115" t="s">
-        <v>10</v>
-      </c>
-      <c r="J9" s="115" t="s">
-        <v>36</v>
-      </c>
       <c r="K9" s="82"/>
     </row>
     <row r="10" spans="1:11" s="71" customFormat="1" ht="12" customHeight="1">
-      <c r="A10" s="115"/>
-      <c r="B10" s="140"/>
-      <c r="C10" s="115"/>
-      <c r="D10" s="135"/>
+      <c r="A10" s="125"/>
+      <c r="B10" s="135"/>
+      <c r="C10" s="125"/>
+      <c r="D10" s="130"/>
       <c r="E10" s="144"/>
       <c r="F10" s="144"/>
       <c r="G10" s="145"/>
-      <c r="H10" s="135"/>
-      <c r="I10" s="115"/>
-      <c r="J10" s="115"/>
+      <c r="H10" s="130"/>
+      <c r="I10" s="125"/>
+      <c r="J10" s="125"/>
       <c r="K10" s="70"/>
     </row>
     <row r="11" spans="1:11" s="84" customFormat="1" ht="15">
-      <c r="A11" s="136"/>
-      <c r="B11" s="136"/>
-      <c r="C11" s="136"/>
-      <c r="D11" s="136"/>
-      <c r="E11" s="136"/>
-      <c r="F11" s="136"/>
-      <c r="G11" s="136"/>
-      <c r="H11" s="136"/>
-      <c r="I11" s="136"/>
-      <c r="J11" s="137"/>
-    </row>
-    <row r="12" spans="1:11" s="4" customFormat="1" ht="13.2">
-      <c r="A12" s="126" t="s">
-        <v>64</v>
-      </c>
-      <c r="B12" s="127"/>
-      <c r="C12" s="127"/>
-      <c r="D12" s="127"/>
-      <c r="E12" s="127"/>
-      <c r="F12" s="127"/>
-      <c r="G12" s="127"/>
-      <c r="H12" s="127"/>
-      <c r="I12" s="127"/>
-      <c r="J12" s="128"/>
-    </row>
-    <row r="13" spans="1:11" s="4" customFormat="1" ht="79.2" outlineLevel="1">
-      <c r="A13" s="88" t="s">
-        <v>3</v>
-      </c>
-      <c r="B13" s="94" t="s">
-        <v>45</v>
-      </c>
-      <c r="C13" s="87" t="s">
-        <v>59</v>
-      </c>
-      <c r="D13" s="119" t="s">
-        <v>48</v>
-      </c>
-      <c r="E13" s="118"/>
-      <c r="F13" s="118"/>
-      <c r="G13" s="86"/>
-      <c r="H13" s="101"/>
-      <c r="I13" s="87" t="s">
-        <v>42</v>
-      </c>
-      <c r="J13" s="85"/>
-    </row>
-    <row r="14" spans="1:11" s="4" customFormat="1" ht="63.75" customHeight="1" outlineLevel="1">
+      <c r="A11" s="131"/>
+      <c r="B11" s="131"/>
+      <c r="C11" s="131"/>
+      <c r="D11" s="131"/>
+      <c r="E11" s="131"/>
+      <c r="F11" s="131"/>
+      <c r="G11" s="131"/>
+      <c r="H11" s="131"/>
+      <c r="I11" s="131"/>
+      <c r="J11" s="132"/>
+    </row>
+    <row r="12" spans="1:11" s="4" customFormat="1" ht="12.75">
+      <c r="A12" s="120" t="s">
+        <v>53</v>
+      </c>
+      <c r="B12" s="121"/>
+      <c r="C12" s="121"/>
+      <c r="D12" s="121"/>
+      <c r="E12" s="121"/>
+      <c r="F12" s="121"/>
+      <c r="G12" s="121"/>
+      <c r="H12" s="121"/>
+      <c r="I12" s="121"/>
+      <c r="J12" s="122"/>
+    </row>
+    <row r="13" spans="1:11" s="4" customFormat="1" ht="12.75">
+      <c r="A13" s="146" t="s">
+        <v>100</v>
+      </c>
+      <c r="B13" s="110"/>
+      <c r="C13" s="110"/>
+      <c r="D13" s="110"/>
+      <c r="E13" s="110"/>
+      <c r="F13" s="110"/>
+      <c r="G13" s="110"/>
+      <c r="H13" s="110"/>
+      <c r="I13" s="110"/>
+      <c r="J13" s="111"/>
+    </row>
+    <row r="14" spans="1:11" s="4" customFormat="1" ht="51" outlineLevel="1">
       <c r="A14" s="88" t="s">
-        <v>4</v>
-      </c>
-      <c r="B14" s="99" t="s">
-        <v>47</v>
-      </c>
-      <c r="C14" s="100" t="s">
-        <v>60</v>
-      </c>
-      <c r="D14" s="116" t="s">
-        <v>2</v>
-      </c>
-      <c r="E14" s="118"/>
-      <c r="F14" s="118"/>
+        <v>54</v>
+      </c>
+      <c r="B14" s="94" t="s">
+        <v>55</v>
+      </c>
+      <c r="C14" s="87" t="s">
+        <v>86</v>
+      </c>
+      <c r="D14" s="140" t="s">
+        <v>56</v>
+      </c>
+      <c r="E14" s="139"/>
+      <c r="F14" s="139"/>
       <c r="G14" s="86"/>
-      <c r="H14" s="96"/>
+      <c r="H14" s="101"/>
       <c r="I14" s="87" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="J14" s="85"/>
     </row>
     <row r="15" spans="1:11" s="4" customFormat="1" ht="63.75" customHeight="1" outlineLevel="1">
       <c r="A15" s="88" t="s">
-        <v>5</v>
-      </c>
-      <c r="B15" s="110" t="s">
-        <v>47</v>
-      </c>
-      <c r="C15" s="87" t="s">
-        <v>61</v>
-      </c>
-      <c r="D15" s="116" t="s">
-        <v>1</v>
-      </c>
-      <c r="E15" s="117"/>
-      <c r="F15" s="117"/>
+        <v>57</v>
+      </c>
+      <c r="B15" s="99" t="s">
+        <v>58</v>
+      </c>
+      <c r="C15" s="100" t="s">
+        <v>85</v>
+      </c>
+      <c r="D15" s="140" t="s">
+        <v>56</v>
+      </c>
+      <c r="E15" s="139"/>
+      <c r="F15" s="139"/>
       <c r="G15" s="86"/>
       <c r="H15" s="96"/>
       <c r="I15" s="87" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="J15" s="85"/>
     </row>
     <row r="16" spans="1:11" s="4" customFormat="1" ht="63.75" customHeight="1" outlineLevel="1">
       <c r="A16" s="88" t="s">
-        <v>5</v>
-      </c>
-      <c r="B16" s="110" t="s">
-        <v>47</v>
+        <v>59</v>
+      </c>
+      <c r="B16" s="108" t="s">
+        <v>75</v>
       </c>
       <c r="C16" s="87" t="s">
-        <v>61</v>
-      </c>
-      <c r="D16" s="116" t="s">
-        <v>1</v>
-      </c>
-      <c r="E16" s="117"/>
-      <c r="F16" s="117"/>
+        <v>60</v>
+      </c>
+      <c r="D16" s="140" t="s">
+        <v>74</v>
+      </c>
+      <c r="E16" s="138"/>
+      <c r="F16" s="138"/>
       <c r="G16" s="86"/>
-      <c r="H16" s="107"/>
+      <c r="H16" s="109"/>
       <c r="I16" s="87" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="J16" s="85"/>
     </row>
     <row r="17" spans="1:10" s="4" customFormat="1" ht="63.75" customHeight="1" outlineLevel="1">
       <c r="A17" s="88" t="s">
-        <v>5</v>
-      </c>
-      <c r="B17" s="110" t="s">
-        <v>47</v>
+        <v>61</v>
+      </c>
+      <c r="B17" s="108" t="s">
+        <v>76</v>
       </c>
       <c r="C17" s="87" t="s">
-        <v>61</v>
-      </c>
-      <c r="D17" s="116" t="s">
+        <v>60</v>
+      </c>
+      <c r="D17" s="140" t="s">
+        <v>74</v>
+      </c>
+      <c r="E17" s="138"/>
+      <c r="F17" s="138"/>
+      <c r="G17" s="86"/>
+      <c r="H17" s="96"/>
+      <c r="I17" s="87" t="s">
+        <v>37</v>
+      </c>
+      <c r="J17" s="85"/>
+    </row>
+    <row r="18" spans="1:10" s="4" customFormat="1" ht="63.75" customHeight="1" outlineLevel="1">
+      <c r="A18" s="88" t="s">
+        <v>64</v>
+      </c>
+      <c r="B18" s="108" t="s">
+        <v>62</v>
+      </c>
+      <c r="C18" s="87" t="s">
+        <v>63</v>
+      </c>
+      <c r="D18" s="140" t="s">
+        <v>56</v>
+      </c>
+      <c r="E18" s="139"/>
+      <c r="F18" s="139"/>
+      <c r="G18" s="86"/>
+      <c r="H18" s="107"/>
+      <c r="I18" s="87" t="s">
+        <v>37</v>
+      </c>
+      <c r="J18" s="85"/>
+    </row>
+    <row r="19" spans="1:10" s="4" customFormat="1" ht="63.75" customHeight="1" outlineLevel="1">
+      <c r="A19" s="88" t="s">
+        <v>72</v>
+      </c>
+      <c r="B19" s="108" t="s">
+        <v>65</v>
+      </c>
+      <c r="C19" s="87" t="s">
+        <v>70</v>
+      </c>
+      <c r="D19" s="140" t="s">
+        <v>68</v>
+      </c>
+      <c r="E19" s="138"/>
+      <c r="F19" s="138"/>
+      <c r="G19" s="86"/>
+      <c r="H19" s="109"/>
+      <c r="I19" s="87" t="s">
+        <v>37</v>
+      </c>
+      <c r="J19" s="85"/>
+    </row>
+    <row r="20" spans="1:10" s="4" customFormat="1" ht="63.75" customHeight="1" outlineLevel="1">
+      <c r="A20" s="88" t="s">
+        <v>73</v>
+      </c>
+      <c r="B20" s="108" t="s">
+        <v>66</v>
+      </c>
+      <c r="C20" s="87" t="s">
+        <v>67</v>
+      </c>
+      <c r="D20" s="140" t="s">
+        <v>68</v>
+      </c>
+      <c r="E20" s="138"/>
+      <c r="F20" s="138"/>
+      <c r="G20" s="86"/>
+      <c r="H20" s="109"/>
+      <c r="I20" s="87" t="s">
+        <v>37</v>
+      </c>
+      <c r="J20" s="85"/>
+    </row>
+    <row r="21" spans="1:10" s="4" customFormat="1" ht="63.75" customHeight="1" outlineLevel="1">
+      <c r="A21" s="88" t="s">
+        <v>77</v>
+      </c>
+      <c r="B21" s="108" t="s">
+        <v>69</v>
+      </c>
+      <c r="C21" s="87" t="s">
+        <v>71</v>
+      </c>
+      <c r="D21" s="140" t="s">
+        <v>68</v>
+      </c>
+      <c r="E21" s="138"/>
+      <c r="F21" s="138"/>
+      <c r="G21" s="86"/>
+      <c r="H21" s="109"/>
+      <c r="I21" s="87" t="s">
+        <v>37</v>
+      </c>
+      <c r="J21" s="85"/>
+    </row>
+    <row r="22" spans="1:10" s="4" customFormat="1" ht="63.75" customHeight="1" outlineLevel="1">
+      <c r="A22" s="88" t="s">
+        <v>78</v>
+      </c>
+      <c r="B22" s="108" t="s">
+        <v>79</v>
+      </c>
+      <c r="C22" s="87" t="s">
+        <v>80</v>
+      </c>
+      <c r="D22" s="140" t="s">
+        <v>81</v>
+      </c>
+      <c r="E22" s="138"/>
+      <c r="F22" s="138"/>
+      <c r="G22" s="86"/>
+      <c r="H22" s="109"/>
+      <c r="I22" s="87" t="s">
+        <v>37</v>
+      </c>
+      <c r="J22" s="85"/>
+    </row>
+    <row r="23" spans="1:10" s="4" customFormat="1" ht="63.75" customHeight="1" outlineLevel="1">
+      <c r="A23" s="88" t="s">
+        <v>82</v>
+      </c>
+      <c r="B23" s="108" t="s">
+        <v>83</v>
+      </c>
+      <c r="C23" s="87" t="s">
+        <v>112</v>
+      </c>
+      <c r="D23" s="140" t="s">
+        <v>74</v>
+      </c>
+      <c r="E23" s="138"/>
+      <c r="F23" s="138"/>
+      <c r="G23" s="86"/>
+      <c r="H23" s="109"/>
+      <c r="I23" s="87" t="s">
+        <v>37</v>
+      </c>
+      <c r="J23" s="85"/>
+    </row>
+    <row r="24" spans="1:10" s="4" customFormat="1" ht="63.75" customHeight="1" outlineLevel="1">
+      <c r="A24" s="88" t="s">
+        <v>95</v>
+      </c>
+      <c r="B24" s="108" t="s">
+        <v>84</v>
+      </c>
+      <c r="C24" s="87" t="s">
+        <v>87</v>
+      </c>
+      <c r="D24" s="140" t="s">
+        <v>68</v>
+      </c>
+      <c r="E24" s="138"/>
+      <c r="F24" s="138"/>
+      <c r="G24" s="86"/>
+      <c r="H24" s="109"/>
+      <c r="I24" s="87" t="s">
+        <v>37</v>
+      </c>
+      <c r="J24" s="85"/>
+    </row>
+    <row r="25" spans="1:10" s="4" customFormat="1" ht="63.75" customHeight="1" outlineLevel="1">
+      <c r="A25" s="88" t="s">
+        <v>96</v>
+      </c>
+      <c r="B25" s="108" t="s">
+        <v>88</v>
+      </c>
+      <c r="C25" s="87" t="s">
+        <v>89</v>
+      </c>
+      <c r="D25" s="140" t="s">
+        <v>68</v>
+      </c>
+      <c r="E25" s="138"/>
+      <c r="F25" s="138"/>
+      <c r="G25" s="86"/>
+      <c r="H25" s="109"/>
+      <c r="I25" s="87" t="s">
+        <v>37</v>
+      </c>
+      <c r="J25" s="85"/>
+    </row>
+    <row r="26" spans="1:10" s="4" customFormat="1" ht="63.75" customHeight="1" outlineLevel="1">
+      <c r="A26" s="88" t="s">
+        <v>97</v>
+      </c>
+      <c r="B26" s="108" t="s">
+        <v>90</v>
+      </c>
+      <c r="C26" s="87" t="s">
+        <v>91</v>
+      </c>
+      <c r="D26" s="140" t="s">
+        <v>68</v>
+      </c>
+      <c r="E26" s="138"/>
+      <c r="F26" s="138"/>
+      <c r="G26" s="86"/>
+      <c r="H26" s="109"/>
+      <c r="I26" s="87" t="s">
+        <v>37</v>
+      </c>
+      <c r="J26" s="85"/>
+    </row>
+    <row r="27" spans="1:10" s="4" customFormat="1" ht="63.75" customHeight="1" outlineLevel="1">
+      <c r="A27" s="88" t="s">
+        <v>98</v>
+      </c>
+      <c r="B27" s="108" t="s">
+        <v>92</v>
+      </c>
+      <c r="C27" s="87" t="s">
+        <v>93</v>
+      </c>
+      <c r="D27" s="140" t="s">
+        <v>94</v>
+      </c>
+      <c r="E27" s="138"/>
+      <c r="F27" s="138"/>
+      <c r="G27" s="86"/>
+      <c r="H27" s="107"/>
+      <c r="I27" s="87" t="s">
         <v>1</v>
       </c>
-      <c r="E17" s="117"/>
-      <c r="F17" s="117"/>
-      <c r="G17" s="86"/>
-      <c r="H17" s="107"/>
-      <c r="I17" s="87" t="s">
-        <v>6</v>
-      </c>
-      <c r="J17" s="85"/>
-    </row>
-    <row r="18" spans="1:10" s="4" customFormat="1" ht="13.2" outlineLevel="1">
-      <c r="A18" s="113" t="s">
-        <v>49</v>
-      </c>
-      <c r="B18" s="114"/>
-      <c r="C18" s="114"/>
-      <c r="D18" s="108"/>
-      <c r="E18" s="108"/>
-      <c r="F18" s="108"/>
-      <c r="G18" s="108"/>
-      <c r="H18" s="108"/>
-      <c r="I18" s="108"/>
-      <c r="J18" s="109"/>
-    </row>
-    <row r="19" spans="1:10" ht="12" customHeight="1"/>
-    <row r="20" spans="1:10" ht="12" customHeight="1"/>
-    <row r="21" spans="1:10" ht="12" customHeight="1"/>
-    <row r="22" spans="1:10" ht="12" customHeight="1"/>
-    <row r="23" spans="1:10" ht="12" customHeight="1"/>
-    <row r="24" spans="1:10" ht="12" customHeight="1"/>
-    <row r="25" spans="1:10" ht="12" customHeight="1"/>
-    <row r="26" spans="1:10" ht="12" customHeight="1"/>
-    <row r="27" spans="1:10" ht="12" customHeight="1"/>
-    <row r="28" spans="1:10" ht="12" customHeight="1"/>
-    <row r="29" spans="1:10" ht="12" customHeight="1"/>
-    <row r="30" spans="1:10" ht="12" customHeight="1"/>
-    <row r="31" spans="1:10" ht="12" customHeight="1"/>
-    <row r="32" spans="1:10" ht="12" customHeight="1"/>
-    <row r="33" ht="12" customHeight="1"/>
-    <row r="34" ht="12" customHeight="1"/>
-    <row r="35" ht="12" customHeight="1"/>
-    <row r="36" ht="12" customHeight="1"/>
-    <row r="37" ht="12" customHeight="1"/>
-    <row r="38" ht="12" customHeight="1"/>
-    <row r="39" ht="12" customHeight="1"/>
-    <row r="40" ht="12" customHeight="1"/>
-    <row r="41" ht="12" customHeight="1"/>
-    <row r="42" ht="12" customHeight="1"/>
-    <row r="43" ht="12" customHeight="1"/>
-    <row r="44" ht="12" customHeight="1"/>
-    <row r="45" ht="12" customHeight="1"/>
-    <row r="46" ht="12" customHeight="1"/>
-    <row r="47" ht="12" customHeight="1"/>
-    <row r="48" ht="12" customHeight="1"/>
+      <c r="J27" s="85"/>
+    </row>
+    <row r="28" spans="1:10" s="4" customFormat="1" ht="12.75">
+      <c r="A28" s="146" t="s">
+        <v>99</v>
+      </c>
+      <c r="B28" s="110"/>
+      <c r="C28" s="110"/>
+      <c r="D28" s="110"/>
+      <c r="E28" s="110"/>
+      <c r="F28" s="110"/>
+      <c r="G28" s="110"/>
+      <c r="H28" s="110"/>
+      <c r="I28" s="110"/>
+      <c r="J28" s="111"/>
+    </row>
+    <row r="29" spans="1:10" s="4" customFormat="1" ht="51" outlineLevel="1">
+      <c r="A29" s="88" t="s">
+        <v>101</v>
+      </c>
+      <c r="B29" s="94" t="s">
+        <v>55</v>
+      </c>
+      <c r="C29" s="87" t="s">
+        <v>102</v>
+      </c>
+      <c r="D29" s="140" t="s">
+        <v>56</v>
+      </c>
+      <c r="E29" s="139"/>
+      <c r="F29" s="139"/>
+      <c r="G29" s="86"/>
+      <c r="H29" s="101"/>
+      <c r="I29" s="87" t="s">
+        <v>37</v>
+      </c>
+      <c r="J29" s="85"/>
+    </row>
+    <row r="30" spans="1:10" s="4" customFormat="1" ht="63.75" customHeight="1" outlineLevel="1">
+      <c r="A30" s="88" t="s">
+        <v>130</v>
+      </c>
+      <c r="B30" s="99" t="s">
+        <v>58</v>
+      </c>
+      <c r="C30" s="100" t="s">
+        <v>103</v>
+      </c>
+      <c r="D30" s="140" t="s">
+        <v>56</v>
+      </c>
+      <c r="E30" s="139"/>
+      <c r="F30" s="139"/>
+      <c r="G30" s="86"/>
+      <c r="H30" s="109"/>
+      <c r="I30" s="87" t="s">
+        <v>37</v>
+      </c>
+      <c r="J30" s="85"/>
+    </row>
+    <row r="31" spans="1:10" s="4" customFormat="1" ht="63.75" customHeight="1" outlineLevel="1">
+      <c r="A31" s="88" t="s">
+        <v>129</v>
+      </c>
+      <c r="B31" s="108" t="s">
+        <v>75</v>
+      </c>
+      <c r="C31" s="87" t="s">
+        <v>104</v>
+      </c>
+      <c r="D31" s="140" t="s">
+        <v>105</v>
+      </c>
+      <c r="E31" s="138"/>
+      <c r="F31" s="138"/>
+      <c r="G31" s="86"/>
+      <c r="H31" s="109"/>
+      <c r="I31" s="87" t="s">
+        <v>110</v>
+      </c>
+      <c r="J31" s="85"/>
+    </row>
+    <row r="32" spans="1:10" s="4" customFormat="1" ht="63.75" customHeight="1" outlineLevel="1">
+      <c r="A32" s="88" t="s">
+        <v>128</v>
+      </c>
+      <c r="B32" s="108" t="s">
+        <v>76</v>
+      </c>
+      <c r="C32" s="87" t="s">
+        <v>104</v>
+      </c>
+      <c r="D32" s="140" t="s">
+        <v>74</v>
+      </c>
+      <c r="E32" s="138"/>
+      <c r="F32" s="138"/>
+      <c r="G32" s="86"/>
+      <c r="H32" s="109"/>
+      <c r="I32" s="87" t="s">
+        <v>37</v>
+      </c>
+      <c r="J32" s="85"/>
+    </row>
+    <row r="33" spans="1:10" s="4" customFormat="1" ht="63.75" customHeight="1" outlineLevel="1">
+      <c r="A33" s="88" t="s">
+        <v>127</v>
+      </c>
+      <c r="B33" s="108" t="s">
+        <v>62</v>
+      </c>
+      <c r="C33" s="87" t="s">
+        <v>106</v>
+      </c>
+      <c r="D33" s="140" t="s">
+        <v>56</v>
+      </c>
+      <c r="E33" s="139"/>
+      <c r="F33" s="139"/>
+      <c r="G33" s="86"/>
+      <c r="H33" s="109"/>
+      <c r="I33" s="87" t="s">
+        <v>37</v>
+      </c>
+      <c r="J33" s="85"/>
+    </row>
+    <row r="34" spans="1:10" s="4" customFormat="1" ht="63.75" customHeight="1" outlineLevel="1">
+      <c r="A34" s="88" t="s">
+        <v>126</v>
+      </c>
+      <c r="B34" s="108" t="s">
+        <v>65</v>
+      </c>
+      <c r="C34" s="87" t="s">
+        <v>107</v>
+      </c>
+      <c r="D34" s="140" t="s">
+        <v>68</v>
+      </c>
+      <c r="E34" s="138"/>
+      <c r="F34" s="138"/>
+      <c r="G34" s="86"/>
+      <c r="H34" s="109"/>
+      <c r="I34" s="87" t="s">
+        <v>37</v>
+      </c>
+      <c r="J34" s="85"/>
+    </row>
+    <row r="35" spans="1:10" s="4" customFormat="1" ht="63.75" customHeight="1" outlineLevel="1">
+      <c r="A35" s="88" t="s">
+        <v>125</v>
+      </c>
+      <c r="B35" s="108" t="s">
+        <v>66</v>
+      </c>
+      <c r="C35" s="87" t="s">
+        <v>108</v>
+      </c>
+      <c r="D35" s="140" t="s">
+        <v>68</v>
+      </c>
+      <c r="E35" s="138"/>
+      <c r="F35" s="138"/>
+      <c r="G35" s="86"/>
+      <c r="H35" s="109"/>
+      <c r="I35" s="87" t="s">
+        <v>37</v>
+      </c>
+      <c r="J35" s="85"/>
+    </row>
+    <row r="36" spans="1:10" s="4" customFormat="1" ht="63.75" customHeight="1" outlineLevel="1">
+      <c r="A36" s="88" t="s">
+        <v>124</v>
+      </c>
+      <c r="B36" s="108" t="s">
+        <v>69</v>
+      </c>
+      <c r="C36" s="87" t="s">
+        <v>109</v>
+      </c>
+      <c r="D36" s="140" t="s">
+        <v>68</v>
+      </c>
+      <c r="E36" s="138"/>
+      <c r="F36" s="138"/>
+      <c r="G36" s="86"/>
+      <c r="H36" s="109"/>
+      <c r="I36" s="87" t="s">
+        <v>37</v>
+      </c>
+      <c r="J36" s="85"/>
+    </row>
+    <row r="37" spans="1:10" s="4" customFormat="1" ht="63.75" customHeight="1" outlineLevel="1">
+      <c r="A37" s="88" t="s">
+        <v>123</v>
+      </c>
+      <c r="B37" s="108" t="s">
+        <v>79</v>
+      </c>
+      <c r="C37" s="87" t="s">
+        <v>111</v>
+      </c>
+      <c r="D37" s="140" t="s">
+        <v>144</v>
+      </c>
+      <c r="E37" s="138"/>
+      <c r="F37" s="138"/>
+      <c r="G37" s="86"/>
+      <c r="H37" s="109"/>
+      <c r="I37" s="87" t="s">
+        <v>110</v>
+      </c>
+      <c r="J37" s="85"/>
+    </row>
+    <row r="38" spans="1:10" s="4" customFormat="1" ht="63.75" customHeight="1" outlineLevel="1">
+      <c r="A38" s="88" t="s">
+        <v>122</v>
+      </c>
+      <c r="B38" s="108" t="s">
+        <v>83</v>
+      </c>
+      <c r="C38" s="87" t="s">
+        <v>113</v>
+      </c>
+      <c r="D38" s="140" t="s">
+        <v>74</v>
+      </c>
+      <c r="E38" s="138"/>
+      <c r="F38" s="138"/>
+      <c r="G38" s="86"/>
+      <c r="H38" s="109"/>
+      <c r="I38" s="87" t="s">
+        <v>37</v>
+      </c>
+      <c r="J38" s="85"/>
+    </row>
+    <row r="39" spans="1:10" s="4" customFormat="1" ht="63.75" customHeight="1" outlineLevel="1">
+      <c r="A39" s="88" t="s">
+        <v>121</v>
+      </c>
+      <c r="B39" s="108" t="s">
+        <v>84</v>
+      </c>
+      <c r="C39" s="87" t="s">
+        <v>114</v>
+      </c>
+      <c r="D39" s="140" t="s">
+        <v>68</v>
+      </c>
+      <c r="E39" s="138"/>
+      <c r="F39" s="138"/>
+      <c r="G39" s="86"/>
+      <c r="H39" s="109"/>
+      <c r="I39" s="87" t="s">
+        <v>37</v>
+      </c>
+      <c r="J39" s="85"/>
+    </row>
+    <row r="40" spans="1:10" s="4" customFormat="1" ht="63.75" customHeight="1" outlineLevel="1">
+      <c r="A40" s="88" t="s">
+        <v>120</v>
+      </c>
+      <c r="B40" s="108" t="s">
+        <v>88</v>
+      </c>
+      <c r="C40" s="87" t="s">
+        <v>115</v>
+      </c>
+      <c r="D40" s="140" t="s">
+        <v>68</v>
+      </c>
+      <c r="E40" s="138"/>
+      <c r="F40" s="138"/>
+      <c r="G40" s="86"/>
+      <c r="H40" s="109"/>
+      <c r="I40" s="87" t="s">
+        <v>37</v>
+      </c>
+      <c r="J40" s="85"/>
+    </row>
+    <row r="41" spans="1:10" s="4" customFormat="1" ht="63.75" customHeight="1" outlineLevel="1">
+      <c r="A41" s="88" t="s">
+        <v>119</v>
+      </c>
+      <c r="B41" s="108" t="s">
+        <v>90</v>
+      </c>
+      <c r="C41" s="87" t="s">
+        <v>116</v>
+      </c>
+      <c r="D41" s="140" t="s">
+        <v>68</v>
+      </c>
+      <c r="E41" s="138"/>
+      <c r="F41" s="138"/>
+      <c r="G41" s="86"/>
+      <c r="H41" s="109"/>
+      <c r="I41" s="87" t="s">
+        <v>37</v>
+      </c>
+      <c r="J41" s="85"/>
+    </row>
+    <row r="42" spans="1:10" s="4" customFormat="1" ht="63.75" customHeight="1" outlineLevel="1">
+      <c r="A42" s="88" t="s">
+        <v>118</v>
+      </c>
+      <c r="B42" s="108" t="s">
+        <v>92</v>
+      </c>
+      <c r="C42" s="87" t="s">
+        <v>117</v>
+      </c>
+      <c r="D42" s="140" t="s">
+        <v>94</v>
+      </c>
+      <c r="E42" s="138"/>
+      <c r="F42" s="138"/>
+      <c r="G42" s="86"/>
+      <c r="H42" s="109"/>
+      <c r="I42" s="87" t="s">
+        <v>1</v>
+      </c>
+      <c r="J42" s="85"/>
+    </row>
+    <row r="43" spans="1:10" ht="12" customHeight="1">
+      <c r="A43" s="120" t="s">
+        <v>131</v>
+      </c>
+      <c r="B43" s="121"/>
+      <c r="C43" s="121"/>
+      <c r="D43" s="121"/>
+      <c r="E43" s="121"/>
+      <c r="F43" s="121"/>
+      <c r="G43" s="121"/>
+      <c r="H43" s="121"/>
+      <c r="I43" s="121"/>
+      <c r="J43" s="122"/>
+    </row>
+    <row r="44" spans="1:10" s="4" customFormat="1" ht="38.25" outlineLevel="1">
+      <c r="A44" s="88" t="s">
+        <v>132</v>
+      </c>
+      <c r="B44" s="94" t="s">
+        <v>133</v>
+      </c>
+      <c r="C44" s="87" t="s">
+        <v>134</v>
+      </c>
+      <c r="D44" s="140" t="s">
+        <v>142</v>
+      </c>
+      <c r="E44" s="139"/>
+      <c r="F44" s="139"/>
+      <c r="G44" s="86"/>
+      <c r="H44" s="101"/>
+      <c r="I44" s="87" t="s">
+        <v>37</v>
+      </c>
+      <c r="J44" s="85"/>
+    </row>
+    <row r="45" spans="1:10" s="4" customFormat="1" ht="38.25" outlineLevel="1">
+      <c r="A45" s="88" t="s">
+        <v>135</v>
+      </c>
+      <c r="B45" s="94" t="s">
+        <v>138</v>
+      </c>
+      <c r="C45" s="87" t="s">
+        <v>136</v>
+      </c>
+      <c r="D45" s="140" t="s">
+        <v>143</v>
+      </c>
+      <c r="E45" s="139"/>
+      <c r="F45" s="139"/>
+      <c r="G45" s="86"/>
+      <c r="H45" s="101"/>
+      <c r="I45" s="87" t="s">
+        <v>37</v>
+      </c>
+      <c r="J45" s="85"/>
+    </row>
+    <row r="46" spans="1:10" s="4" customFormat="1" ht="38.25" outlineLevel="1">
+      <c r="A46" s="88" t="s">
+        <v>140</v>
+      </c>
+      <c r="B46" s="94" t="s">
+        <v>137</v>
+      </c>
+      <c r="C46" s="87" t="s">
+        <v>139</v>
+      </c>
+      <c r="D46" s="140" t="s">
+        <v>141</v>
+      </c>
+      <c r="E46" s="139"/>
+      <c r="F46" s="139"/>
+      <c r="G46" s="86"/>
+      <c r="H46" s="101"/>
+      <c r="I46" s="87" t="s">
+        <v>37</v>
+      </c>
+      <c r="J46" s="85"/>
+    </row>
+    <row r="47" spans="1:10" ht="12" customHeight="1">
+      <c r="A47" s="136" t="s">
+        <v>41</v>
+      </c>
+      <c r="B47" s="137"/>
+      <c r="C47" s="137"/>
+      <c r="D47" s="110"/>
+      <c r="E47" s="110"/>
+      <c r="F47" s="110"/>
+      <c r="G47" s="110"/>
+      <c r="H47" s="110"/>
+      <c r="I47" s="110"/>
+      <c r="J47" s="111"/>
+    </row>
+    <row r="48" spans="1:10" ht="12" customHeight="1"/>
     <row r="49" ht="12" customHeight="1"/>
     <row r="50" ht="12" customHeight="1"/>
     <row r="51" ht="12" customHeight="1"/>
     <row r="52" ht="12" customHeight="1"/>
     <row r="53" ht="12" customHeight="1"/>
+    <row r="54" ht="12" customHeight="1"/>
+    <row r="55" ht="12" customHeight="1"/>
+    <row r="56" ht="12" customHeight="1"/>
+    <row r="57" ht="12" customHeight="1"/>
+    <row r="58" ht="12" customHeight="1"/>
+    <row r="59" ht="12" customHeight="1"/>
+    <row r="60" ht="12" customHeight="1"/>
+    <row r="61" ht="12" customHeight="1"/>
+    <row r="62" ht="12" customHeight="1"/>
+    <row r="63" ht="12" customHeight="1"/>
+    <row r="64" ht="12" customHeight="1"/>
+    <row r="65" ht="12" customHeight="1"/>
+    <row r="66" ht="12" customHeight="1"/>
+    <row r="67" ht="12" customHeight="1"/>
+    <row r="68" ht="12" customHeight="1"/>
+    <row r="69" ht="12" customHeight="1"/>
+    <row r="70" ht="12" customHeight="1"/>
+    <row r="71" ht="12" customHeight="1"/>
+    <row r="72" ht="12" customHeight="1"/>
+    <row r="73" ht="12" customHeight="1"/>
+    <row r="74" ht="12" customHeight="1"/>
+    <row r="75" ht="12" customHeight="1"/>
+    <row r="76" ht="12" customHeight="1"/>
+    <row r="77" ht="12" customHeight="1"/>
+    <row r="78" ht="12" customHeight="1"/>
+    <row r="79" ht="12" customHeight="1"/>
+    <row r="80" ht="12" customHeight="1"/>
   </sheetData>
-  <mergeCells count="25">
+  <mergeCells count="52">
+    <mergeCell ref="D44:F44"/>
+    <mergeCell ref="D45:F45"/>
+    <mergeCell ref="D46:F46"/>
+    <mergeCell ref="D39:F39"/>
+    <mergeCell ref="D40:F40"/>
+    <mergeCell ref="D41:F41"/>
+    <mergeCell ref="D42:F42"/>
+    <mergeCell ref="A43:J43"/>
+    <mergeCell ref="D34:F34"/>
+    <mergeCell ref="D35:F35"/>
+    <mergeCell ref="D36:F36"/>
+    <mergeCell ref="D37:F37"/>
+    <mergeCell ref="D38:F38"/>
+    <mergeCell ref="D29:F29"/>
+    <mergeCell ref="D30:F30"/>
+    <mergeCell ref="D31:F31"/>
+    <mergeCell ref="D32:F32"/>
+    <mergeCell ref="D33:F33"/>
+    <mergeCell ref="D19:F19"/>
+    <mergeCell ref="D21:F21"/>
+    <mergeCell ref="D16:F16"/>
+    <mergeCell ref="A47:C47"/>
+    <mergeCell ref="I9:I10"/>
+    <mergeCell ref="D17:F17"/>
+    <mergeCell ref="D18:F18"/>
+    <mergeCell ref="D27:F27"/>
+    <mergeCell ref="D15:F15"/>
+    <mergeCell ref="D14:F14"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D9:G10"/>
+    <mergeCell ref="D20:F20"/>
+    <mergeCell ref="D22:F22"/>
+    <mergeCell ref="D23:F23"/>
+    <mergeCell ref="D24:F24"/>
+    <mergeCell ref="D25:F25"/>
+    <mergeCell ref="D26:F26"/>
     <mergeCell ref="B1:D2"/>
     <mergeCell ref="A8:D8"/>
     <mergeCell ref="B5:D5"/>
@@ -2435,15 +3303,6 @@
     <mergeCell ref="A11:J11"/>
     <mergeCell ref="A9:A10"/>
     <mergeCell ref="B9:B10"/>
-    <mergeCell ref="A18:C18"/>
-    <mergeCell ref="I9:I10"/>
-    <mergeCell ref="D15:F15"/>
-    <mergeCell ref="D16:F16"/>
-    <mergeCell ref="D17:F17"/>
-    <mergeCell ref="D14:F14"/>
-    <mergeCell ref="D13:F13"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D9:G10"/>
   </mergeCells>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2460,15 +3319,15 @@
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="13.5"/>
   <cols>
-    <col min="3" max="3" width="22.77734375" customWidth="1"/>
-    <col min="7" max="7" width="18.77734375" customWidth="1"/>
+    <col min="3" max="3" width="22.75" customWidth="1"/>
+    <col min="7" max="7" width="18.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="22.2">
+    <row r="1" spans="1:7" ht="22.5">
       <c r="A1" s="15" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B1" s="16"/>
       <c r="C1" s="17"/>
@@ -2486,9 +3345,9 @@
       <c r="F2" s="17"/>
       <c r="G2" s="18"/>
     </row>
-    <row r="3" spans="1:7" ht="13.8">
+    <row r="3" spans="1:7" ht="14.25">
       <c r="B3" s="19" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C3" s="17"/>
       <c r="D3" s="17"/>
@@ -2496,9 +3355,9 @@
       <c r="F3" s="17"/>
       <c r="G3" s="18"/>
     </row>
-    <row r="4" spans="1:7" ht="13.8">
+    <row r="4" spans="1:7" ht="14.25">
       <c r="B4" s="19" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C4" s="103"/>
       <c r="D4" s="19"/>
@@ -2506,7 +3365,7 @@
       <c r="F4" s="19"/>
       <c r="G4" s="19"/>
     </row>
-    <row r="5" spans="1:7" ht="13.8">
+    <row r="5" spans="1:7" ht="14.25">
       <c r="A5" s="19"/>
       <c r="B5" s="19"/>
       <c r="C5" s="19"/>
@@ -2515,7 +3374,7 @@
       <c r="F5" s="19"/>
       <c r="G5" s="19"/>
     </row>
-    <row r="6" spans="1:7" ht="13.8">
+    <row r="6" spans="1:7" ht="14.25">
       <c r="A6" s="19"/>
       <c r="B6" s="19"/>
       <c r="C6" s="19"/>
@@ -2524,28 +3383,28 @@
       <c r="F6" s="19"/>
       <c r="G6" s="19"/>
     </row>
-    <row r="7" spans="1:7" ht="26.4">
+    <row r="7" spans="1:7" ht="25.5">
       <c r="A7" s="20"/>
       <c r="B7" s="55" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C7" s="56" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="D7" s="57" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="E7" s="56" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="F7" s="56" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="G7" s="58" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" s="67" customFormat="1" ht="13.8">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" s="67" customFormat="1" ht="14.25">
       <c r="A8" s="73"/>
       <c r="B8" s="74">
         <v>1</v>
@@ -2556,7 +3415,7 @@
       </c>
       <c r="D8" s="76">
         <f>Samples!B6</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E8" s="75">
         <f>Samples!B7</f>
@@ -2568,10 +3427,10 @@
       </c>
       <c r="G8" s="76">
         <f>Samples!D7</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="13.8">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="14.25">
       <c r="A9" s="19"/>
       <c r="B9" s="34"/>
       <c r="C9" s="33"/>
@@ -2580,15 +3439,15 @@
       <c r="F9" s="32"/>
       <c r="G9" s="35"/>
     </row>
-    <row r="10" spans="1:7" ht="13.8">
+    <row r="10" spans="1:7" ht="14.25">
       <c r="A10" s="19"/>
       <c r="B10" s="59"/>
       <c r="C10" s="60" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="D10" s="61">
         <f>SUM(D6:D9)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E10" s="61">
         <f>SUM(E6:E9)</f>
@@ -2600,10 +3459,10 @@
       </c>
       <c r="G10" s="62">
         <f>SUM(G6:G9)</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="13.8">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="14.25">
       <c r="A11" s="19"/>
       <c r="B11" s="21"/>
       <c r="C11" s="19"/>
@@ -2612,35 +3471,35 @@
       <c r="F11" s="23"/>
       <c r="G11" s="23"/>
     </row>
-    <row r="12" spans="1:7" ht="13.8">
+    <row r="12" spans="1:7" ht="14.25">
       <c r="A12" s="19"/>
       <c r="B12" s="19"/>
       <c r="C12" s="19" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D12" s="19"/>
       <c r="E12" s="24">
         <f>(D10+E10)*100/G10</f>
-        <v>166.66666666666666</v>
+        <v>46.153846153846153</v>
       </c>
       <c r="F12" s="19" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="G12" s="25"/>
     </row>
-    <row r="13" spans="1:7" ht="13.8">
+    <row r="13" spans="1:7" ht="14.25">
       <c r="A13" s="19"/>
       <c r="B13" s="19"/>
       <c r="C13" s="19" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="D13" s="19"/>
       <c r="E13" s="24">
         <f>D10*100/G10</f>
-        <v>133.33333333333334</v>
+        <v>38.46153846153846</v>
       </c>
       <c r="F13" s="19" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="G13" s="25"/>
     </row>

</xml_diff>

<commit_message>
cap nhat link test-case
</commit_message>
<xml_diff>
--- a/test-case-example.xlsx
+++ b/test-case-example.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23426"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Khoa Pham\Documents\kiemthu\QuanLyThuVien\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\qltv\QuanLyThuVien\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{618E6794-CC06-4056-87F5-B7A61AC58F6B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="821" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="821"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="97" r:id="rId1"/>
@@ -30,12 +29,12 @@
     <definedName name="Port">[1]Validation!$F$2:$F$40</definedName>
     <definedName name="VancoProducts">[1]Validation!$B$2:$B$4</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="180">
   <si>
     <t>31/07/2007</t>
   </si>
@@ -185,9 +184,6 @@
     <t>CR236 "Export all carrier choices"</t>
   </si>
   <si>
-    <t>Check set Role CanExportAllCarrierChoices = False</t>
-  </si>
-  <si>
     <t>1.1</t>
   </si>
   <si>
@@ -558,11 +554,129 @@
   <si>
     <t>Hiện ra giao diện NhanVienGUI</t>
   </si>
+  <si>
+    <t>3. Kiểm tra thông tin form TheDocGia</t>
+  </si>
+  <si>
+    <t>TDG1</t>
+  </si>
+  <si>
+    <t>Kiểm tra thông tin Độc giả</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1: Vào database kiểm tra thông tin Độc giả
+</t>
+  </si>
+  <si>
+    <t>Thẻ hiện thông tin đúng</t>
+  </si>
+  <si>
+    <t>TDG2</t>
+  </si>
+  <si>
+    <t>Kiểm tra nút Trở về</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1: Click vào nút Trở về
+</t>
+  </si>
+  <si>
+    <t>4. Kiểm tra form TraCuuSach</t>
+  </si>
+  <si>
+    <t>TCS1</t>
+  </si>
+  <si>
+    <t>TCS2</t>
+  </si>
+  <si>
+    <t>TCS3</t>
+  </si>
+  <si>
+    <t>Tra cứu đúng theo Tên sách</t>
+  </si>
+  <si>
+    <t>Tra cứu Tên sách bằng chữ thường</t>
+  </si>
+  <si>
+    <t>Tra cứu Tên sách bằng chữ in hoa</t>
+  </si>
+  <si>
+    <t>TCS4</t>
+  </si>
+  <si>
+    <t>Tra cứu Tác giả</t>
+  </si>
+  <si>
+    <t>Tra cứu Tác giả bằng chữ thường</t>
+  </si>
+  <si>
+    <t>TCS5</t>
+  </si>
+  <si>
+    <t>TCS6</t>
+  </si>
+  <si>
+    <t>Tra cứu Tác giả bằng chữ in hoa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1: Nhập Tác giả cần tìm bằng chữ in hoa
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1: Nhập Tác giả cần tìm bằng chữ thường
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1: Nhập chính xác Tác giả
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1: Nhập chính xác Tên sách cần tìm
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1: Nhập Tên sách cần tìm bằng chữ thường
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1: Nhập Tên sách cần tìm bằng chữ in hoa
+</t>
+  </si>
+  <si>
+    <t>Hiện ra đúng với Tác giả đã nhập</t>
+  </si>
+  <si>
+    <t>Hiện ra đúng với Tên sách đã nhập</t>
+  </si>
+  <si>
+    <t>TCS7</t>
+  </si>
+  <si>
+    <t>Tra cứu chính xác theo Năm xuất bản</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1: Nhập chính xác Năm xuất bản cần tìm
+</t>
+  </si>
+  <si>
+    <t>Hiện ra đúng với Năm xuất bản đã nhập</t>
+  </si>
+  <si>
+    <t>TCS8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+</t>
+  </si>
+  <si>
+    <t>TCS9</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="[$-409]d\-mmm\-yy;@"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
@@ -1216,7 +1330,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="147">
+  <cellXfs count="150">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -1495,12 +1609,69 @@
     <xf numFmtId="0" fontId="22" fillId="4" borderId="17" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="22" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="17" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="20" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="23" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="24" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="20" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="22" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="17" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="20" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="22" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="30" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="31" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="32" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="27" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="33" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="34" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1519,24 +1690,12 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="25" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="20" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="22" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="17" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="20" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1549,9 +1708,6 @@
     <xf numFmtId="0" fontId="15" fillId="5" borderId="26" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="27" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="20" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1559,53 +1715,20 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="5" borderId="30" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="30" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="5" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="20" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="22" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="31" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="32" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="33" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="34" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="20" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal_Functional Test Case v1.0" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
-    <cellStyle name="Normal_Sheet1_Vanco_CR022a1_TestCase_v0.1" xfId="2" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
-    <cellStyle name="標準_結合試験(AllOvertheWorld)" xfId="3" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Normal_Functional Test Case v1.0" xfId="1"/>
+    <cellStyle name="Normal_Sheet1_Vanco_CR022a1_TestCase_v0.1" xfId="2"/>
+    <cellStyle name="標準_結合試験(AllOvertheWorld)" xfId="3"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1709,23 +1832,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1761,23 +1867,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1953,23 +2042,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H23"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8"/>
   <cols>
     <col min="1" max="1" width="9" style="1"/>
-    <col min="2" max="2" width="14.125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="14.109375" style="1" customWidth="1"/>
     <col min="3" max="3" width="9" style="1"/>
     <col min="4" max="4" width="15" style="1" customWidth="1"/>
-    <col min="5" max="5" width="32.5" style="1" customWidth="1"/>
-    <col min="6" max="6" width="23.75" style="1" customWidth="1"/>
-    <col min="7" max="7" width="20.5" style="1" customWidth="1"/>
-    <col min="8" max="8" width="26.625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="32.44140625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="23.77734375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="20.44140625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="26.6640625" style="1" customWidth="1"/>
     <col min="9" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
@@ -1977,7 +2066,7 @@
       <c r="B1" s="31"/>
       <c r="C1" s="31"/>
     </row>
-    <row r="2" spans="1:8" ht="22.5">
+    <row r="2" spans="1:8" ht="22.2">
       <c r="A2" s="26"/>
       <c r="B2" s="27" t="s">
         <v>3</v>
@@ -2014,7 +2103,7 @@
       <c r="F4" s="26"/>
       <c r="G4" s="26"/>
     </row>
-    <row r="5" spans="1:8" ht="15" thickBot="1">
+    <row r="5" spans="1:8" ht="14.4" thickBot="1">
       <c r="A5" s="26"/>
       <c r="B5" s="28"/>
       <c r="C5" s="29"/>
@@ -2028,11 +2117,11 @@
       <c r="B6" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="C6" s="112" t="s">
-        <v>45</v>
-      </c>
-      <c r="D6" s="112"/>
-      <c r="E6" s="113"/>
+      <c r="C6" s="115" t="s">
+        <v>44</v>
+      </c>
+      <c r="D6" s="115"/>
+      <c r="E6" s="116"/>
       <c r="F6" s="26"/>
       <c r="G6" s="26"/>
     </row>
@@ -2041,11 +2130,11 @@
       <c r="B7" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="C7" s="112" t="s">
-        <v>46</v>
-      </c>
-      <c r="D7" s="112"/>
-      <c r="E7" s="113"/>
+      <c r="C7" s="115" t="s">
+        <v>45</v>
+      </c>
+      <c r="D7" s="115"/>
+      <c r="E7" s="116"/>
       <c r="F7" s="26"/>
       <c r="G7" s="26"/>
     </row>
@@ -2072,7 +2161,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:8" s="36" customFormat="1" ht="25.5">
+    <row r="11" spans="1:8" s="36" customFormat="1" ht="26.4">
       <c r="B11" s="52" t="s">
         <v>10</v>
       </c>
@@ -2095,7 +2184,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:8" s="36" customFormat="1">
+    <row r="12" spans="1:8" s="36" customFormat="1" ht="26.4">
       <c r="B12" s="38">
         <v>39293</v>
       </c>
@@ -2107,56 +2196,56 @@
         <v>11</v>
       </c>
       <c r="F12" s="77" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G12" s="89"/>
       <c r="H12" s="91" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:8" s="36" customFormat="1">
+    <row r="13" spans="1:8" s="36" customFormat="1" ht="26.4">
       <c r="B13" s="103">
         <v>39295</v>
       </c>
       <c r="C13" s="39" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D13" s="40"/>
       <c r="E13" s="41" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F13" s="77" t="s">
+        <v>50</v>
+      </c>
+      <c r="G13" s="102" t="s">
         <v>51</v>
-      </c>
-      <c r="G13" s="102" t="s">
-        <v>52</v>
       </c>
       <c r="H13" s="91" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:8" s="37" customFormat="1" ht="12.75">
+    <row r="14" spans="1:8" s="37" customFormat="1" ht="26.4">
       <c r="B14" s="38">
         <v>39311</v>
       </c>
       <c r="C14" s="39" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D14" s="40"/>
       <c r="E14" s="41" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F14" s="77" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G14" s="102" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H14" s="91" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:8" s="37" customFormat="1" ht="12.75">
+    <row r="15" spans="1:8" s="37" customFormat="1" ht="13.2">
       <c r="B15" s="45"/>
       <c r="C15" s="46"/>
       <c r="D15" s="43"/>
@@ -2252,24 +2341,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:K80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="H47" sqref="H47"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="14.25" outlineLevelRow="1"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8" outlineLevelRow="1"/>
   <cols>
-    <col min="1" max="1" width="15.625" customWidth="1"/>
-    <col min="2" max="2" width="18.125" style="95" customWidth="1"/>
-    <col min="3" max="3" width="42.125" customWidth="1"/>
-    <col min="6" max="6" width="23.625" customWidth="1"/>
-    <col min="7" max="7" width="18.5" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="17.125" customWidth="1"/>
+    <col min="1" max="1" width="15.6640625" customWidth="1"/>
+    <col min="2" max="2" width="18.109375" style="95" customWidth="1"/>
+    <col min="3" max="3" width="42.109375" customWidth="1"/>
+    <col min="6" max="6" width="23.6640625" customWidth="1"/>
+    <col min="7" max="7" width="18.44140625" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="17.109375" customWidth="1"/>
     <col min="9" max="9" width="9" style="98"/>
     <col min="10" max="10" width="18" style="97" customWidth="1"/>
   </cols>
@@ -2278,9 +2367,9 @@
       <c r="A1" s="64" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="114"/>
-      <c r="C1" s="114"/>
-      <c r="D1" s="114"/>
+      <c r="B1" s="133"/>
+      <c r="C1" s="133"/>
+      <c r="D1" s="133"/>
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
       <c r="G1" s="6"/>
@@ -2291,9 +2380,9 @@
     </row>
     <row r="2" spans="1:11" s="2" customFormat="1" ht="11.25" customHeight="1" thickBot="1">
       <c r="A2" s="7"/>
-      <c r="B2" s="115"/>
-      <c r="C2" s="115"/>
-      <c r="D2" s="115"/>
+      <c r="B2" s="134"/>
+      <c r="C2" s="134"/>
+      <c r="D2" s="134"/>
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
@@ -2306,51 +2395,51 @@
       <c r="A3" s="65" t="s">
         <v>35</v>
       </c>
-      <c r="B3" s="112" t="s">
-        <v>48</v>
-      </c>
-      <c r="C3" s="112"/>
-      <c r="D3" s="113"/>
+      <c r="B3" s="115" t="s">
+        <v>47</v>
+      </c>
+      <c r="C3" s="115"/>
+      <c r="D3" s="116"/>
       <c r="E3" s="68"/>
       <c r="F3" s="68"/>
       <c r="G3" s="68"/>
-      <c r="H3" s="124"/>
-      <c r="I3" s="124"/>
-      <c r="J3" s="124"/>
+      <c r="H3" s="140"/>
+      <c r="I3" s="140"/>
+      <c r="J3" s="140"/>
       <c r="K3" s="9"/>
     </row>
-    <row r="4" spans="1:11" s="3" customFormat="1" ht="12.75">
+    <row r="4" spans="1:11" s="3" customFormat="1" ht="13.2">
       <c r="A4" s="72" t="s">
         <v>36</v>
       </c>
-      <c r="B4" s="126" t="s">
-        <v>49</v>
-      </c>
-      <c r="C4" s="127"/>
-      <c r="D4" s="128"/>
+      <c r="B4" s="141" t="s">
+        <v>48</v>
+      </c>
+      <c r="C4" s="142"/>
+      <c r="D4" s="143"/>
       <c r="E4" s="68"/>
       <c r="F4" s="68"/>
       <c r="G4" s="68"/>
-      <c r="H4" s="124"/>
-      <c r="I4" s="124"/>
-      <c r="J4" s="124"/>
+      <c r="H4" s="140"/>
+      <c r="I4" s="140"/>
+      <c r="J4" s="140"/>
       <c r="K4" s="9"/>
     </row>
-    <row r="5" spans="1:11" s="81" customFormat="1" ht="12.75">
+    <row r="5" spans="1:11" s="81" customFormat="1" ht="26.4">
       <c r="A5" s="72" t="s">
         <v>29</v>
       </c>
-      <c r="B5" s="117" t="s">
-        <v>50</v>
-      </c>
-      <c r="C5" s="118"/>
-      <c r="D5" s="119"/>
+      <c r="B5" s="136" t="s">
+        <v>49</v>
+      </c>
+      <c r="C5" s="137"/>
+      <c r="D5" s="138"/>
       <c r="E5" s="79"/>
       <c r="F5" s="79"/>
       <c r="G5" s="79"/>
-      <c r="H5" s="123"/>
-      <c r="I5" s="123"/>
-      <c r="J5" s="123"/>
+      <c r="H5" s="139"/>
+      <c r="I5" s="139"/>
+      <c r="J5" s="139"/>
       <c r="K5" s="80"/>
     </row>
     <row r="6" spans="1:11" s="3" customFormat="1" ht="15" customHeight="1">
@@ -2371,9 +2460,9 @@
       <c r="E6" s="8"/>
       <c r="F6" s="8"/>
       <c r="G6" s="8"/>
-      <c r="H6" s="124"/>
-      <c r="I6" s="124"/>
-      <c r="J6" s="124"/>
+      <c r="H6" s="140"/>
+      <c r="I6" s="140"/>
+      <c r="J6" s="140"/>
       <c r="K6" s="9"/>
     </row>
     <row r="7" spans="1:11" s="3" customFormat="1" ht="15" customHeight="1" thickBot="1">
@@ -2394,16 +2483,16 @@
       <c r="E7" s="69"/>
       <c r="F7" s="69"/>
       <c r="G7" s="69"/>
-      <c r="H7" s="124"/>
-      <c r="I7" s="124"/>
-      <c r="J7" s="124"/>
+      <c r="H7" s="140"/>
+      <c r="I7" s="140"/>
+      <c r="J7" s="140"/>
       <c r="K7" s="9"/>
     </row>
     <row r="8" spans="1:11" s="3" customFormat="1" ht="15" customHeight="1">
-      <c r="A8" s="116"/>
-      <c r="B8" s="116"/>
-      <c r="C8" s="116"/>
-      <c r="D8" s="116"/>
+      <c r="A8" s="135"/>
+      <c r="B8" s="135"/>
+      <c r="C8" s="135"/>
+      <c r="D8" s="135"/>
       <c r="E8" s="8"/>
       <c r="F8" s="8"/>
       <c r="G8" s="8"/>
@@ -2413,22 +2502,22 @@
       <c r="K8" s="9"/>
     </row>
     <row r="9" spans="1:11" s="83" customFormat="1" ht="12" customHeight="1">
-      <c r="A9" s="133" t="s">
+      <c r="A9" s="126" t="s">
         <v>30</v>
       </c>
-      <c r="B9" s="134" t="s">
+      <c r="B9" s="147" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="133" t="s">
+      <c r="C9" s="126" t="s">
         <v>15</v>
       </c>
-      <c r="D9" s="141" t="s">
+      <c r="D9" s="127" t="s">
         <v>28</v>
       </c>
-      <c r="E9" s="142"/>
-      <c r="F9" s="142"/>
-      <c r="G9" s="143"/>
-      <c r="H9" s="129" t="s">
+      <c r="E9" s="128"/>
+      <c r="F9" s="128"/>
+      <c r="G9" s="129"/>
+      <c r="H9" s="144" t="s">
         <v>26</v>
       </c>
       <c r="I9" s="125" t="s">
@@ -2441,32 +2530,32 @@
     </row>
     <row r="10" spans="1:11" s="71" customFormat="1" ht="12" customHeight="1">
       <c r="A10" s="125"/>
-      <c r="B10" s="135"/>
+      <c r="B10" s="148"/>
       <c r="C10" s="125"/>
       <c r="D10" s="130"/>
-      <c r="E10" s="144"/>
-      <c r="F10" s="144"/>
-      <c r="G10" s="145"/>
+      <c r="E10" s="131"/>
+      <c r="F10" s="131"/>
+      <c r="G10" s="132"/>
       <c r="H10" s="130"/>
       <c r="I10" s="125"/>
       <c r="J10" s="125"/>
       <c r="K10" s="70"/>
     </row>
     <row r="11" spans="1:11" s="84" customFormat="1" ht="15">
-      <c r="A11" s="131"/>
-      <c r="B11" s="131"/>
-      <c r="C11" s="131"/>
-      <c r="D11" s="131"/>
-      <c r="E11" s="131"/>
-      <c r="F11" s="131"/>
-      <c r="G11" s="131"/>
-      <c r="H11" s="131"/>
-      <c r="I11" s="131"/>
-      <c r="J11" s="132"/>
-    </row>
-    <row r="12" spans="1:11" s="4" customFormat="1" ht="12.75">
+      <c r="A11" s="145"/>
+      <c r="B11" s="145"/>
+      <c r="C11" s="145"/>
+      <c r="D11" s="145"/>
+      <c r="E11" s="145"/>
+      <c r="F11" s="145"/>
+      <c r="G11" s="145"/>
+      <c r="H11" s="145"/>
+      <c r="I11" s="145"/>
+      <c r="J11" s="146"/>
+    </row>
+    <row r="12" spans="1:11" s="4" customFormat="1" ht="13.2">
       <c r="A12" s="120" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B12" s="121"/>
       <c r="C12" s="121"/>
@@ -2478,9 +2567,9 @@
       <c r="I12" s="121"/>
       <c r="J12" s="122"/>
     </row>
-    <row r="13" spans="1:11" s="4" customFormat="1" ht="12.75">
-      <c r="A13" s="146" t="s">
-        <v>100</v>
+    <row r="13" spans="1:11" s="4" customFormat="1" ht="13.2">
+      <c r="A13" s="114" t="s">
+        <v>99</v>
       </c>
       <c r="B13" s="110"/>
       <c r="C13" s="110"/>
@@ -2492,21 +2581,21 @@
       <c r="I13" s="110"/>
       <c r="J13" s="111"/>
     </row>
-    <row r="14" spans="1:11" s="4" customFormat="1" ht="51" outlineLevel="1">
+    <row r="14" spans="1:11" s="4" customFormat="1" ht="52.8" outlineLevel="1">
       <c r="A14" s="88" t="s">
+        <v>53</v>
+      </c>
+      <c r="B14" s="94" t="s">
         <v>54</v>
       </c>
-      <c r="B14" s="94" t="s">
+      <c r="C14" s="87" t="s">
+        <v>85</v>
+      </c>
+      <c r="D14" s="117" t="s">
         <v>55</v>
       </c>
-      <c r="C14" s="87" t="s">
-        <v>86</v>
-      </c>
-      <c r="D14" s="140" t="s">
-        <v>56</v>
-      </c>
-      <c r="E14" s="139"/>
-      <c r="F14" s="139"/>
+      <c r="E14" s="118"/>
+      <c r="F14" s="118"/>
       <c r="G14" s="86"/>
       <c r="H14" s="101"/>
       <c r="I14" s="87" t="s">
@@ -2516,19 +2605,19 @@
     </row>
     <row r="15" spans="1:11" s="4" customFormat="1" ht="63.75" customHeight="1" outlineLevel="1">
       <c r="A15" s="88" t="s">
+        <v>56</v>
+      </c>
+      <c r="B15" s="149" t="s">
         <v>57</v>
       </c>
-      <c r="B15" s="99" t="s">
-        <v>58</v>
-      </c>
       <c r="C15" s="100" t="s">
-        <v>85</v>
-      </c>
-      <c r="D15" s="140" t="s">
-        <v>56</v>
-      </c>
-      <c r="E15" s="139"/>
-      <c r="F15" s="139"/>
+        <v>84</v>
+      </c>
+      <c r="D15" s="117" t="s">
+        <v>55</v>
+      </c>
+      <c r="E15" s="118"/>
+      <c r="F15" s="118"/>
       <c r="G15" s="86"/>
       <c r="H15" s="96"/>
       <c r="I15" s="87" t="s">
@@ -2538,19 +2627,19 @@
     </row>
     <row r="16" spans="1:11" s="4" customFormat="1" ht="63.75" customHeight="1" outlineLevel="1">
       <c r="A16" s="88" t="s">
+        <v>58</v>
+      </c>
+      <c r="B16" s="94" t="s">
+        <v>74</v>
+      </c>
+      <c r="C16" s="87" t="s">
         <v>59</v>
       </c>
-      <c r="B16" s="108" t="s">
-        <v>75</v>
-      </c>
-      <c r="C16" s="87" t="s">
-        <v>60</v>
-      </c>
-      <c r="D16" s="140" t="s">
-        <v>74</v>
-      </c>
-      <c r="E16" s="138"/>
-      <c r="F16" s="138"/>
+      <c r="D16" s="117" t="s">
+        <v>73</v>
+      </c>
+      <c r="E16" s="119"/>
+      <c r="F16" s="119"/>
       <c r="G16" s="86"/>
       <c r="H16" s="109"/>
       <c r="I16" s="87" t="s">
@@ -2558,21 +2647,21 @@
       </c>
       <c r="J16" s="85"/>
     </row>
-    <row r="17" spans="1:10" s="4" customFormat="1" ht="63.75" customHeight="1" outlineLevel="1">
+    <row r="17" spans="1:10" s="4" customFormat="1" ht="66.599999999999994" customHeight="1" outlineLevel="1">
       <c r="A17" s="88" t="s">
-        <v>61</v>
-      </c>
-      <c r="B17" s="108" t="s">
-        <v>76</v>
+        <v>60</v>
+      </c>
+      <c r="B17" s="94" t="s">
+        <v>75</v>
       </c>
       <c r="C17" s="87" t="s">
-        <v>60</v>
-      </c>
-      <c r="D17" s="140" t="s">
-        <v>74</v>
-      </c>
-      <c r="E17" s="138"/>
-      <c r="F17" s="138"/>
+        <v>59</v>
+      </c>
+      <c r="D17" s="117" t="s">
+        <v>73</v>
+      </c>
+      <c r="E17" s="119"/>
+      <c r="F17" s="119"/>
       <c r="G17" s="86"/>
       <c r="H17" s="96"/>
       <c r="I17" s="87" t="s">
@@ -2582,19 +2671,19 @@
     </row>
     <row r="18" spans="1:10" s="4" customFormat="1" ht="63.75" customHeight="1" outlineLevel="1">
       <c r="A18" s="88" t="s">
-        <v>64</v>
-      </c>
-      <c r="B18" s="108" t="s">
+        <v>63</v>
+      </c>
+      <c r="B18" s="94" t="s">
+        <v>61</v>
+      </c>
+      <c r="C18" s="87" t="s">
         <v>62</v>
       </c>
-      <c r="C18" s="87" t="s">
-        <v>63</v>
-      </c>
-      <c r="D18" s="140" t="s">
-        <v>56</v>
-      </c>
-      <c r="E18" s="139"/>
-      <c r="F18" s="139"/>
+      <c r="D18" s="117" t="s">
+        <v>55</v>
+      </c>
+      <c r="E18" s="118"/>
+      <c r="F18" s="118"/>
       <c r="G18" s="86"/>
       <c r="H18" s="107"/>
       <c r="I18" s="87" t="s">
@@ -2604,19 +2693,19 @@
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1" ht="63.75" customHeight="1" outlineLevel="1">
       <c r="A19" s="88" t="s">
-        <v>72</v>
-      </c>
-      <c r="B19" s="108" t="s">
-        <v>65</v>
+        <v>71</v>
+      </c>
+      <c r="B19" s="94" t="s">
+        <v>64</v>
       </c>
       <c r="C19" s="87" t="s">
-        <v>70</v>
-      </c>
-      <c r="D19" s="140" t="s">
-        <v>68</v>
-      </c>
-      <c r="E19" s="138"/>
-      <c r="F19" s="138"/>
+        <v>69</v>
+      </c>
+      <c r="D19" s="117" t="s">
+        <v>67</v>
+      </c>
+      <c r="E19" s="119"/>
+      <c r="F19" s="119"/>
       <c r="G19" s="86"/>
       <c r="H19" s="109"/>
       <c r="I19" s="87" t="s">
@@ -2626,19 +2715,19 @@
     </row>
     <row r="20" spans="1:10" s="4" customFormat="1" ht="63.75" customHeight="1" outlineLevel="1">
       <c r="A20" s="88" t="s">
-        <v>73</v>
-      </c>
-      <c r="B20" s="108" t="s">
+        <v>72</v>
+      </c>
+      <c r="B20" s="94" t="s">
+        <v>65</v>
+      </c>
+      <c r="C20" s="87" t="s">
         <v>66</v>
       </c>
-      <c r="C20" s="87" t="s">
+      <c r="D20" s="117" t="s">
         <v>67</v>
       </c>
-      <c r="D20" s="140" t="s">
-        <v>68</v>
-      </c>
-      <c r="E20" s="138"/>
-      <c r="F20" s="138"/>
+      <c r="E20" s="119"/>
+      <c r="F20" s="119"/>
       <c r="G20" s="86"/>
       <c r="H20" s="109"/>
       <c r="I20" s="87" t="s">
@@ -2648,19 +2737,19 @@
     </row>
     <row r="21" spans="1:10" s="4" customFormat="1" ht="63.75" customHeight="1" outlineLevel="1">
       <c r="A21" s="88" t="s">
-        <v>77</v>
-      </c>
-      <c r="B21" s="108" t="s">
-        <v>69</v>
+        <v>76</v>
+      </c>
+      <c r="B21" s="94" t="s">
+        <v>68</v>
       </c>
       <c r="C21" s="87" t="s">
-        <v>71</v>
-      </c>
-      <c r="D21" s="140" t="s">
-        <v>68</v>
-      </c>
-      <c r="E21" s="138"/>
-      <c r="F21" s="138"/>
+        <v>70</v>
+      </c>
+      <c r="D21" s="117" t="s">
+        <v>67</v>
+      </c>
+      <c r="E21" s="119"/>
+      <c r="F21" s="119"/>
       <c r="G21" s="86"/>
       <c r="H21" s="109"/>
       <c r="I21" s="87" t="s">
@@ -2670,19 +2759,19 @@
     </row>
     <row r="22" spans="1:10" s="4" customFormat="1" ht="63.75" customHeight="1" outlineLevel="1">
       <c r="A22" s="88" t="s">
+        <v>77</v>
+      </c>
+      <c r="B22" s="94" t="s">
         <v>78</v>
       </c>
-      <c r="B22" s="108" t="s">
+      <c r="C22" s="87" t="s">
         <v>79</v>
       </c>
-      <c r="C22" s="87" t="s">
+      <c r="D22" s="117" t="s">
         <v>80</v>
       </c>
-      <c r="D22" s="140" t="s">
-        <v>81</v>
-      </c>
-      <c r="E22" s="138"/>
-      <c r="F22" s="138"/>
+      <c r="E22" s="119"/>
+      <c r="F22" s="119"/>
       <c r="G22" s="86"/>
       <c r="H22" s="109"/>
       <c r="I22" s="87" t="s">
@@ -2692,19 +2781,19 @@
     </row>
     <row r="23" spans="1:10" s="4" customFormat="1" ht="63.75" customHeight="1" outlineLevel="1">
       <c r="A23" s="88" t="s">
+        <v>81</v>
+      </c>
+      <c r="B23" s="94" t="s">
         <v>82</v>
       </c>
-      <c r="B23" s="108" t="s">
-        <v>83</v>
-      </c>
       <c r="C23" s="87" t="s">
-        <v>112</v>
-      </c>
-      <c r="D23" s="140" t="s">
-        <v>74</v>
-      </c>
-      <c r="E23" s="138"/>
-      <c r="F23" s="138"/>
+        <v>111</v>
+      </c>
+      <c r="D23" s="117" t="s">
+        <v>73</v>
+      </c>
+      <c r="E23" s="119"/>
+      <c r="F23" s="119"/>
       <c r="G23" s="86"/>
       <c r="H23" s="109"/>
       <c r="I23" s="87" t="s">
@@ -2714,19 +2803,19 @@
     </row>
     <row r="24" spans="1:10" s="4" customFormat="1" ht="63.75" customHeight="1" outlineLevel="1">
       <c r="A24" s="88" t="s">
-        <v>95</v>
-      </c>
-      <c r="B24" s="108" t="s">
-        <v>84</v>
+        <v>94</v>
+      </c>
+      <c r="B24" s="94" t="s">
+        <v>83</v>
       </c>
       <c r="C24" s="87" t="s">
-        <v>87</v>
-      </c>
-      <c r="D24" s="140" t="s">
-        <v>68</v>
-      </c>
-      <c r="E24" s="138"/>
-      <c r="F24" s="138"/>
+        <v>86</v>
+      </c>
+      <c r="D24" s="117" t="s">
+        <v>67</v>
+      </c>
+      <c r="E24" s="119"/>
+      <c r="F24" s="119"/>
       <c r="G24" s="86"/>
       <c r="H24" s="109"/>
       <c r="I24" s="87" t="s">
@@ -2736,19 +2825,19 @@
     </row>
     <row r="25" spans="1:10" s="4" customFormat="1" ht="63.75" customHeight="1" outlineLevel="1">
       <c r="A25" s="88" t="s">
-        <v>96</v>
-      </c>
-      <c r="B25" s="108" t="s">
+        <v>95</v>
+      </c>
+      <c r="B25" s="94" t="s">
+        <v>87</v>
+      </c>
+      <c r="C25" s="87" t="s">
         <v>88</v>
       </c>
-      <c r="C25" s="87" t="s">
-        <v>89</v>
-      </c>
-      <c r="D25" s="140" t="s">
-        <v>68</v>
-      </c>
-      <c r="E25" s="138"/>
-      <c r="F25" s="138"/>
+      <c r="D25" s="117" t="s">
+        <v>67</v>
+      </c>
+      <c r="E25" s="119"/>
+      <c r="F25" s="119"/>
       <c r="G25" s="86"/>
       <c r="H25" s="109"/>
       <c r="I25" s="87" t="s">
@@ -2758,19 +2847,19 @@
     </row>
     <row r="26" spans="1:10" s="4" customFormat="1" ht="63.75" customHeight="1" outlineLevel="1">
       <c r="A26" s="88" t="s">
-        <v>97</v>
-      </c>
-      <c r="B26" s="108" t="s">
+        <v>96</v>
+      </c>
+      <c r="B26" s="94" t="s">
+        <v>89</v>
+      </c>
+      <c r="C26" s="87" t="s">
         <v>90</v>
       </c>
-      <c r="C26" s="87" t="s">
-        <v>91</v>
-      </c>
-      <c r="D26" s="140" t="s">
-        <v>68</v>
-      </c>
-      <c r="E26" s="138"/>
-      <c r="F26" s="138"/>
+      <c r="D26" s="117" t="s">
+        <v>67</v>
+      </c>
+      <c r="E26" s="119"/>
+      <c r="F26" s="119"/>
       <c r="G26" s="86"/>
       <c r="H26" s="109"/>
       <c r="I26" s="87" t="s">
@@ -2780,19 +2869,19 @@
     </row>
     <row r="27" spans="1:10" s="4" customFormat="1" ht="63.75" customHeight="1" outlineLevel="1">
       <c r="A27" s="88" t="s">
-        <v>98</v>
-      </c>
-      <c r="B27" s="108" t="s">
+        <v>97</v>
+      </c>
+      <c r="B27" s="94" t="s">
+        <v>91</v>
+      </c>
+      <c r="C27" s="87" t="s">
         <v>92</v>
       </c>
-      <c r="C27" s="87" t="s">
+      <c r="D27" s="117" t="s">
         <v>93</v>
       </c>
-      <c r="D27" s="140" t="s">
-        <v>94</v>
-      </c>
-      <c r="E27" s="138"/>
-      <c r="F27" s="138"/>
+      <c r="E27" s="119"/>
+      <c r="F27" s="119"/>
       <c r="G27" s="86"/>
       <c r="H27" s="107"/>
       <c r="I27" s="87" t="s">
@@ -2800,9 +2889,9 @@
       </c>
       <c r="J27" s="85"/>
     </row>
-    <row r="28" spans="1:10" s="4" customFormat="1" ht="12.75">
-      <c r="A28" s="146" t="s">
-        <v>99</v>
+    <row r="28" spans="1:10" s="4" customFormat="1" ht="13.2">
+      <c r="A28" s="114" t="s">
+        <v>98</v>
       </c>
       <c r="B28" s="110"/>
       <c r="C28" s="110"/>
@@ -2814,21 +2903,21 @@
       <c r="I28" s="110"/>
       <c r="J28" s="111"/>
     </row>
-    <row r="29" spans="1:10" s="4" customFormat="1" ht="51" outlineLevel="1">
+    <row r="29" spans="1:10" s="4" customFormat="1" ht="52.8" outlineLevel="1">
       <c r="A29" s="88" t="s">
+        <v>100</v>
+      </c>
+      <c r="B29" s="94" t="s">
+        <v>54</v>
+      </c>
+      <c r="C29" s="87" t="s">
         <v>101</v>
       </c>
-      <c r="B29" s="94" t="s">
+      <c r="D29" s="117" t="s">
         <v>55</v>
       </c>
-      <c r="C29" s="87" t="s">
-        <v>102</v>
-      </c>
-      <c r="D29" s="140" t="s">
-        <v>56</v>
-      </c>
-      <c r="E29" s="139"/>
-      <c r="F29" s="139"/>
+      <c r="E29" s="118"/>
+      <c r="F29" s="118"/>
       <c r="G29" s="86"/>
       <c r="H29" s="101"/>
       <c r="I29" s="87" t="s">
@@ -2838,19 +2927,19 @@
     </row>
     <row r="30" spans="1:10" s="4" customFormat="1" ht="63.75" customHeight="1" outlineLevel="1">
       <c r="A30" s="88" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B30" s="99" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C30" s="100" t="s">
-        <v>103</v>
-      </c>
-      <c r="D30" s="140" t="s">
-        <v>56</v>
-      </c>
-      <c r="E30" s="139"/>
-      <c r="F30" s="139"/>
+        <v>102</v>
+      </c>
+      <c r="D30" s="117" t="s">
+        <v>55</v>
+      </c>
+      <c r="E30" s="118"/>
+      <c r="F30" s="118"/>
       <c r="G30" s="86"/>
       <c r="H30" s="109"/>
       <c r="I30" s="87" t="s">
@@ -2860,41 +2949,41 @@
     </row>
     <row r="31" spans="1:10" s="4" customFormat="1" ht="63.75" customHeight="1" outlineLevel="1">
       <c r="A31" s="88" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B31" s="108" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C31" s="87" t="s">
+        <v>103</v>
+      </c>
+      <c r="D31" s="117" t="s">
         <v>104</v>
       </c>
-      <c r="D31" s="140" t="s">
-        <v>105</v>
-      </c>
-      <c r="E31" s="138"/>
-      <c r="F31" s="138"/>
+      <c r="E31" s="119"/>
+      <c r="F31" s="119"/>
       <c r="G31" s="86"/>
       <c r="H31" s="109"/>
       <c r="I31" s="87" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="J31" s="85"/>
     </row>
     <row r="32" spans="1:10" s="4" customFormat="1" ht="63.75" customHeight="1" outlineLevel="1">
       <c r="A32" s="88" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B32" s="108" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C32" s="87" t="s">
-        <v>104</v>
-      </c>
-      <c r="D32" s="140" t="s">
-        <v>74</v>
-      </c>
-      <c r="E32" s="138"/>
-      <c r="F32" s="138"/>
+        <v>103</v>
+      </c>
+      <c r="D32" s="117" t="s">
+        <v>73</v>
+      </c>
+      <c r="E32" s="119"/>
+      <c r="F32" s="119"/>
       <c r="G32" s="86"/>
       <c r="H32" s="109"/>
       <c r="I32" s="87" t="s">
@@ -2904,19 +2993,19 @@
     </row>
     <row r="33" spans="1:10" s="4" customFormat="1" ht="63.75" customHeight="1" outlineLevel="1">
       <c r="A33" s="88" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B33" s="108" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C33" s="87" t="s">
-        <v>106</v>
-      </c>
-      <c r="D33" s="140" t="s">
-        <v>56</v>
-      </c>
-      <c r="E33" s="139"/>
-      <c r="F33" s="139"/>
+        <v>105</v>
+      </c>
+      <c r="D33" s="117" t="s">
+        <v>55</v>
+      </c>
+      <c r="E33" s="118"/>
+      <c r="F33" s="118"/>
       <c r="G33" s="86"/>
       <c r="H33" s="109"/>
       <c r="I33" s="87" t="s">
@@ -2926,19 +3015,19 @@
     </row>
     <row r="34" spans="1:10" s="4" customFormat="1" ht="63.75" customHeight="1" outlineLevel="1">
       <c r="A34" s="88" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B34" s="108" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C34" s="87" t="s">
-        <v>107</v>
-      </c>
-      <c r="D34" s="140" t="s">
-        <v>68</v>
-      </c>
-      <c r="E34" s="138"/>
-      <c r="F34" s="138"/>
+        <v>106</v>
+      </c>
+      <c r="D34" s="117" t="s">
+        <v>67</v>
+      </c>
+      <c r="E34" s="119"/>
+      <c r="F34" s="119"/>
       <c r="G34" s="86"/>
       <c r="H34" s="109"/>
       <c r="I34" s="87" t="s">
@@ -2948,19 +3037,19 @@
     </row>
     <row r="35" spans="1:10" s="4" customFormat="1" ht="63.75" customHeight="1" outlineLevel="1">
       <c r="A35" s="88" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B35" s="108" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C35" s="87" t="s">
-        <v>108</v>
-      </c>
-      <c r="D35" s="140" t="s">
-        <v>68</v>
-      </c>
-      <c r="E35" s="138"/>
-      <c r="F35" s="138"/>
+        <v>107</v>
+      </c>
+      <c r="D35" s="117" t="s">
+        <v>67</v>
+      </c>
+      <c r="E35" s="119"/>
+      <c r="F35" s="119"/>
       <c r="G35" s="86"/>
       <c r="H35" s="109"/>
       <c r="I35" s="87" t="s">
@@ -2970,19 +3059,19 @@
     </row>
     <row r="36" spans="1:10" s="4" customFormat="1" ht="63.75" customHeight="1" outlineLevel="1">
       <c r="A36" s="88" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B36" s="108" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C36" s="87" t="s">
-        <v>109</v>
-      </c>
-      <c r="D36" s="140" t="s">
-        <v>68</v>
-      </c>
-      <c r="E36" s="138"/>
-      <c r="F36" s="138"/>
+        <v>108</v>
+      </c>
+      <c r="D36" s="117" t="s">
+        <v>67</v>
+      </c>
+      <c r="E36" s="119"/>
+      <c r="F36" s="119"/>
       <c r="G36" s="86"/>
       <c r="H36" s="109"/>
       <c r="I36" s="87" t="s">
@@ -2992,41 +3081,41 @@
     </row>
     <row r="37" spans="1:10" s="4" customFormat="1" ht="63.75" customHeight="1" outlineLevel="1">
       <c r="A37" s="88" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B37" s="108" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C37" s="87" t="s">
-        <v>111</v>
-      </c>
-      <c r="D37" s="140" t="s">
-        <v>144</v>
-      </c>
-      <c r="E37" s="138"/>
-      <c r="F37" s="138"/>
+        <v>110</v>
+      </c>
+      <c r="D37" s="117" t="s">
+        <v>143</v>
+      </c>
+      <c r="E37" s="119"/>
+      <c r="F37" s="119"/>
       <c r="G37" s="86"/>
       <c r="H37" s="109"/>
       <c r="I37" s="87" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="J37" s="85"/>
     </row>
     <row r="38" spans="1:10" s="4" customFormat="1" ht="63.75" customHeight="1" outlineLevel="1">
       <c r="A38" s="88" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B38" s="108" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C38" s="87" t="s">
-        <v>113</v>
-      </c>
-      <c r="D38" s="140" t="s">
-        <v>74</v>
-      </c>
-      <c r="E38" s="138"/>
-      <c r="F38" s="138"/>
+        <v>112</v>
+      </c>
+      <c r="D38" s="117" t="s">
+        <v>73</v>
+      </c>
+      <c r="E38" s="119"/>
+      <c r="F38" s="119"/>
       <c r="G38" s="86"/>
       <c r="H38" s="109"/>
       <c r="I38" s="87" t="s">
@@ -3036,19 +3125,19 @@
     </row>
     <row r="39" spans="1:10" s="4" customFormat="1" ht="63.75" customHeight="1" outlineLevel="1">
       <c r="A39" s="88" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B39" s="108" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C39" s="87" t="s">
-        <v>114</v>
-      </c>
-      <c r="D39" s="140" t="s">
-        <v>68</v>
-      </c>
-      <c r="E39" s="138"/>
-      <c r="F39" s="138"/>
+        <v>113</v>
+      </c>
+      <c r="D39" s="117" t="s">
+        <v>67</v>
+      </c>
+      <c r="E39" s="119"/>
+      <c r="F39" s="119"/>
       <c r="G39" s="86"/>
       <c r="H39" s="109"/>
       <c r="I39" s="87" t="s">
@@ -3058,19 +3147,19 @@
     </row>
     <row r="40" spans="1:10" s="4" customFormat="1" ht="63.75" customHeight="1" outlineLevel="1">
       <c r="A40" s="88" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B40" s="108" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C40" s="87" t="s">
-        <v>115</v>
-      </c>
-      <c r="D40" s="140" t="s">
-        <v>68</v>
-      </c>
-      <c r="E40" s="138"/>
-      <c r="F40" s="138"/>
+        <v>114</v>
+      </c>
+      <c r="D40" s="117" t="s">
+        <v>67</v>
+      </c>
+      <c r="E40" s="119"/>
+      <c r="F40" s="119"/>
       <c r="G40" s="86"/>
       <c r="H40" s="109"/>
       <c r="I40" s="87" t="s">
@@ -3080,19 +3169,19 @@
     </row>
     <row r="41" spans="1:10" s="4" customFormat="1" ht="63.75" customHeight="1" outlineLevel="1">
       <c r="A41" s="88" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B41" s="108" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C41" s="87" t="s">
-        <v>116</v>
-      </c>
-      <c r="D41" s="140" t="s">
-        <v>68</v>
-      </c>
-      <c r="E41" s="138"/>
-      <c r="F41" s="138"/>
+        <v>115</v>
+      </c>
+      <c r="D41" s="117" t="s">
+        <v>67</v>
+      </c>
+      <c r="E41" s="119"/>
+      <c r="F41" s="119"/>
       <c r="G41" s="86"/>
       <c r="H41" s="109"/>
       <c r="I41" s="87" t="s">
@@ -3102,19 +3191,19 @@
     </row>
     <row r="42" spans="1:10" s="4" customFormat="1" ht="63.75" customHeight="1" outlineLevel="1">
       <c r="A42" s="88" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B42" s="108" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C42" s="87" t="s">
-        <v>117</v>
-      </c>
-      <c r="D42" s="140" t="s">
-        <v>94</v>
-      </c>
-      <c r="E42" s="138"/>
-      <c r="F42" s="138"/>
+        <v>116</v>
+      </c>
+      <c r="D42" s="117" t="s">
+        <v>93</v>
+      </c>
+      <c r="E42" s="119"/>
+      <c r="F42" s="119"/>
       <c r="G42" s="86"/>
       <c r="H42" s="109"/>
       <c r="I42" s="87" t="s">
@@ -3124,7 +3213,7 @@
     </row>
     <row r="43" spans="1:10" ht="12" customHeight="1">
       <c r="A43" s="120" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B43" s="121"/>
       <c r="C43" s="121"/>
@@ -3136,21 +3225,21 @@
       <c r="I43" s="121"/>
       <c r="J43" s="122"/>
     </row>
-    <row r="44" spans="1:10" s="4" customFormat="1" ht="38.25" outlineLevel="1">
+    <row r="44" spans="1:10" s="4" customFormat="1" ht="39.6" outlineLevel="1">
       <c r="A44" s="88" t="s">
+        <v>131</v>
+      </c>
+      <c r="B44" s="94" t="s">
         <v>132</v>
       </c>
-      <c r="B44" s="94" t="s">
+      <c r="C44" s="87" t="s">
         <v>133</v>
       </c>
-      <c r="C44" s="87" t="s">
-        <v>134</v>
-      </c>
-      <c r="D44" s="140" t="s">
-        <v>142</v>
-      </c>
-      <c r="E44" s="139"/>
-      <c r="F44" s="139"/>
+      <c r="D44" s="117" t="s">
+        <v>141</v>
+      </c>
+      <c r="E44" s="118"/>
+      <c r="F44" s="118"/>
       <c r="G44" s="86"/>
       <c r="H44" s="101"/>
       <c r="I44" s="87" t="s">
@@ -3158,21 +3247,21 @@
       </c>
       <c r="J44" s="85"/>
     </row>
-    <row r="45" spans="1:10" s="4" customFormat="1" ht="38.25" outlineLevel="1">
+    <row r="45" spans="1:10" s="4" customFormat="1" ht="39.6" outlineLevel="1">
       <c r="A45" s="88" t="s">
+        <v>134</v>
+      </c>
+      <c r="B45" s="94" t="s">
+        <v>137</v>
+      </c>
+      <c r="C45" s="87" t="s">
         <v>135</v>
       </c>
-      <c r="B45" s="94" t="s">
-        <v>138</v>
-      </c>
-      <c r="C45" s="87" t="s">
-        <v>136</v>
-      </c>
-      <c r="D45" s="140" t="s">
-        <v>143</v>
-      </c>
-      <c r="E45" s="139"/>
-      <c r="F45" s="139"/>
+      <c r="D45" s="117" t="s">
+        <v>142</v>
+      </c>
+      <c r="E45" s="118"/>
+      <c r="F45" s="118"/>
       <c r="G45" s="86"/>
       <c r="H45" s="101"/>
       <c r="I45" s="87" t="s">
@@ -3180,21 +3269,21 @@
       </c>
       <c r="J45" s="85"/>
     </row>
-    <row r="46" spans="1:10" s="4" customFormat="1" ht="38.25" outlineLevel="1">
+    <row r="46" spans="1:10" s="4" customFormat="1" ht="39.6" outlineLevel="1">
       <c r="A46" s="88" t="s">
+        <v>139</v>
+      </c>
+      <c r="B46" s="94" t="s">
+        <v>136</v>
+      </c>
+      <c r="C46" s="87" t="s">
+        <v>138</v>
+      </c>
+      <c r="D46" s="117" t="s">
         <v>140</v>
       </c>
-      <c r="B46" s="94" t="s">
-        <v>137</v>
-      </c>
-      <c r="C46" s="87" t="s">
-        <v>139</v>
-      </c>
-      <c r="D46" s="140" t="s">
-        <v>141</v>
-      </c>
-      <c r="E46" s="139"/>
-      <c r="F46" s="139"/>
+      <c r="E46" s="118"/>
+      <c r="F46" s="118"/>
       <c r="G46" s="86"/>
       <c r="H46" s="101"/>
       <c r="I46" s="87" t="s">
@@ -3203,11 +3292,11 @@
       <c r="J46" s="85"/>
     </row>
     <row r="47" spans="1:10" ht="12" customHeight="1">
-      <c r="A47" s="136" t="s">
-        <v>41</v>
-      </c>
-      <c r="B47" s="137"/>
-      <c r="C47" s="137"/>
+      <c r="A47" s="123" t="s">
+        <v>144</v>
+      </c>
+      <c r="B47" s="124"/>
+      <c r="C47" s="124"/>
       <c r="D47" s="110"/>
       <c r="E47" s="110"/>
       <c r="F47" s="110"/>
@@ -3216,23 +3305,255 @@
       <c r="I47" s="110"/>
       <c r="J47" s="111"/>
     </row>
-    <row r="48" spans="1:10" ht="12" customHeight="1"/>
-    <row r="49" ht="12" customHeight="1"/>
-    <row r="50" ht="12" customHeight="1"/>
-    <row r="51" ht="12" customHeight="1"/>
-    <row r="52" ht="12" customHeight="1"/>
-    <row r="53" ht="12" customHeight="1"/>
-    <row r="54" ht="12" customHeight="1"/>
-    <row r="55" ht="12" customHeight="1"/>
-    <row r="56" ht="12" customHeight="1"/>
-    <row r="57" ht="12" customHeight="1"/>
-    <row r="58" ht="12" customHeight="1"/>
-    <row r="59" ht="12" customHeight="1"/>
-    <row r="60" ht="12" customHeight="1"/>
-    <row r="61" ht="12" customHeight="1"/>
-    <row r="62" ht="12" customHeight="1"/>
-    <row r="63" ht="12" customHeight="1"/>
-    <row r="64" ht="12" customHeight="1"/>
+    <row r="48" spans="1:10" s="4" customFormat="1" ht="39.6" outlineLevel="1">
+      <c r="A48" s="88" t="s">
+        <v>145</v>
+      </c>
+      <c r="B48" s="94" t="s">
+        <v>146</v>
+      </c>
+      <c r="C48" s="87" t="s">
+        <v>147</v>
+      </c>
+      <c r="D48" s="117" t="s">
+        <v>148</v>
+      </c>
+      <c r="E48" s="118"/>
+      <c r="F48" s="118"/>
+      <c r="G48" s="86"/>
+      <c r="H48" s="101"/>
+      <c r="I48" s="87" t="s">
+        <v>37</v>
+      </c>
+      <c r="J48" s="85"/>
+    </row>
+    <row r="49" spans="1:10" s="4" customFormat="1" ht="39.6" outlineLevel="1">
+      <c r="A49" s="88" t="s">
+        <v>149</v>
+      </c>
+      <c r="B49" s="94" t="s">
+        <v>150</v>
+      </c>
+      <c r="C49" s="87" t="s">
+        <v>151</v>
+      </c>
+      <c r="D49" s="117" t="s">
+        <v>80</v>
+      </c>
+      <c r="E49" s="118"/>
+      <c r="F49" s="118"/>
+      <c r="G49" s="86"/>
+      <c r="H49" s="101"/>
+      <c r="I49" s="87" t="s">
+        <v>37</v>
+      </c>
+      <c r="J49" s="85"/>
+    </row>
+    <row r="50" spans="1:10" ht="12" customHeight="1">
+      <c r="A50" s="123" t="s">
+        <v>152</v>
+      </c>
+      <c r="B50" s="124"/>
+      <c r="C50" s="124"/>
+      <c r="D50" s="112"/>
+      <c r="E50" s="112"/>
+      <c r="F50" s="112"/>
+      <c r="G50" s="112"/>
+      <c r="H50" s="112"/>
+      <c r="I50" s="112"/>
+      <c r="J50" s="113"/>
+    </row>
+    <row r="51" spans="1:10" s="4" customFormat="1" ht="39.6" outlineLevel="1">
+      <c r="A51" s="88" t="s">
+        <v>153</v>
+      </c>
+      <c r="B51" s="94" t="s">
+        <v>156</v>
+      </c>
+      <c r="C51" s="87" t="s">
+        <v>168</v>
+      </c>
+      <c r="D51" s="117" t="s">
+        <v>172</v>
+      </c>
+      <c r="E51" s="118"/>
+      <c r="F51" s="118"/>
+      <c r="G51" s="86"/>
+      <c r="H51" s="101"/>
+      <c r="I51" s="87" t="s">
+        <v>37</v>
+      </c>
+      <c r="J51" s="85"/>
+    </row>
+    <row r="52" spans="1:10" s="4" customFormat="1" ht="39.6" outlineLevel="1">
+      <c r="A52" s="88" t="s">
+        <v>154</v>
+      </c>
+      <c r="B52" s="94" t="s">
+        <v>157</v>
+      </c>
+      <c r="C52" s="87" t="s">
+        <v>169</v>
+      </c>
+      <c r="D52" s="117" t="s">
+        <v>172</v>
+      </c>
+      <c r="E52" s="118"/>
+      <c r="F52" s="118"/>
+      <c r="G52" s="86"/>
+      <c r="H52" s="101"/>
+      <c r="I52" s="87" t="s">
+        <v>37</v>
+      </c>
+      <c r="J52" s="85"/>
+    </row>
+    <row r="53" spans="1:10" s="4" customFormat="1" ht="39.6" outlineLevel="1">
+      <c r="A53" s="88" t="s">
+        <v>155</v>
+      </c>
+      <c r="B53" s="94" t="s">
+        <v>158</v>
+      </c>
+      <c r="C53" s="87" t="s">
+        <v>170</v>
+      </c>
+      <c r="D53" s="117" t="s">
+        <v>172</v>
+      </c>
+      <c r="E53" s="118"/>
+      <c r="F53" s="118"/>
+      <c r="G53" s="86"/>
+      <c r="H53" s="101"/>
+      <c r="I53" s="87" t="s">
+        <v>37</v>
+      </c>
+      <c r="J53" s="85"/>
+    </row>
+    <row r="54" spans="1:10" s="4" customFormat="1" ht="39.6" outlineLevel="1">
+      <c r="A54" s="88" t="s">
+        <v>159</v>
+      </c>
+      <c r="B54" s="94" t="s">
+        <v>160</v>
+      </c>
+      <c r="C54" s="87" t="s">
+        <v>167</v>
+      </c>
+      <c r="D54" s="117" t="s">
+        <v>171</v>
+      </c>
+      <c r="E54" s="118"/>
+      <c r="F54" s="118"/>
+      <c r="G54" s="86"/>
+      <c r="H54" s="101"/>
+      <c r="I54" s="87" t="s">
+        <v>37</v>
+      </c>
+      <c r="J54" s="85"/>
+    </row>
+    <row r="55" spans="1:10" s="4" customFormat="1" ht="39.6" outlineLevel="1">
+      <c r="A55" s="88" t="s">
+        <v>162</v>
+      </c>
+      <c r="B55" s="94" t="s">
+        <v>161</v>
+      </c>
+      <c r="C55" s="87" t="s">
+        <v>166</v>
+      </c>
+      <c r="D55" s="117" t="s">
+        <v>171</v>
+      </c>
+      <c r="E55" s="118"/>
+      <c r="F55" s="118"/>
+      <c r="G55" s="86"/>
+      <c r="H55" s="101"/>
+      <c r="I55" s="87" t="s">
+        <v>37</v>
+      </c>
+      <c r="J55" s="85"/>
+    </row>
+    <row r="56" spans="1:10" s="4" customFormat="1" ht="39.6" outlineLevel="1">
+      <c r="A56" s="88" t="s">
+        <v>163</v>
+      </c>
+      <c r="B56" s="94" t="s">
+        <v>164</v>
+      </c>
+      <c r="C56" s="87" t="s">
+        <v>165</v>
+      </c>
+      <c r="D56" s="117" t="s">
+        <v>171</v>
+      </c>
+      <c r="E56" s="118"/>
+      <c r="F56" s="118"/>
+      <c r="G56" s="86"/>
+      <c r="H56" s="101"/>
+      <c r="I56" s="87" t="s">
+        <v>37</v>
+      </c>
+      <c r="J56" s="85"/>
+    </row>
+    <row r="57" spans="1:10" s="4" customFormat="1" ht="39.6" outlineLevel="1">
+      <c r="A57" s="88" t="s">
+        <v>173</v>
+      </c>
+      <c r="B57" s="94" t="s">
+        <v>174</v>
+      </c>
+      <c r="C57" s="87" t="s">
+        <v>175</v>
+      </c>
+      <c r="D57" s="117" t="s">
+        <v>176</v>
+      </c>
+      <c r="E57" s="118"/>
+      <c r="F57" s="118"/>
+      <c r="G57" s="86"/>
+      <c r="H57" s="101"/>
+      <c r="I57" s="87" t="s">
+        <v>37</v>
+      </c>
+      <c r="J57" s="85"/>
+    </row>
+    <row r="58" spans="1:10" s="4" customFormat="1" ht="39.6" outlineLevel="1">
+      <c r="A58" s="88" t="s">
+        <v>177</v>
+      </c>
+      <c r="B58" s="94"/>
+      <c r="C58" s="87" t="s">
+        <v>178</v>
+      </c>
+      <c r="D58" s="117"/>
+      <c r="E58" s="118"/>
+      <c r="F58" s="118"/>
+      <c r="G58" s="86"/>
+      <c r="H58" s="101"/>
+      <c r="I58" s="87"/>
+      <c r="J58" s="85"/>
+    </row>
+    <row r="59" spans="1:10" s="4" customFormat="1" ht="39.6" outlineLevel="1">
+      <c r="A59" s="88" t="s">
+        <v>179</v>
+      </c>
+      <c r="B59" s="94"/>
+      <c r="C59" s="87" t="s">
+        <v>178</v>
+      </c>
+      <c r="D59" s="117"/>
+      <c r="E59" s="118"/>
+      <c r="F59" s="118"/>
+      <c r="G59" s="86"/>
+      <c r="H59" s="101"/>
+      <c r="I59" s="87"/>
+      <c r="J59" s="85"/>
+    </row>
+    <row r="60" spans="1:10" ht="12" customHeight="1"/>
+    <row r="61" spans="1:10" ht="12" customHeight="1"/>
+    <row r="62" spans="1:10" ht="12" customHeight="1"/>
+    <row r="63" spans="1:10" ht="12" customHeight="1"/>
+    <row r="64" spans="1:10" ht="12" customHeight="1"/>
     <row r="65" ht="12" customHeight="1"/>
     <row r="66" ht="12" customHeight="1"/>
     <row r="67" ht="12" customHeight="1"/>
@@ -3250,25 +3571,37 @@
     <row r="79" ht="12" customHeight="1"/>
     <row r="80" ht="12" customHeight="1"/>
   </sheetData>
-  <mergeCells count="52">
-    <mergeCell ref="D44:F44"/>
-    <mergeCell ref="D45:F45"/>
-    <mergeCell ref="D46:F46"/>
-    <mergeCell ref="D39:F39"/>
-    <mergeCell ref="D40:F40"/>
-    <mergeCell ref="D41:F41"/>
-    <mergeCell ref="D42:F42"/>
-    <mergeCell ref="A43:J43"/>
-    <mergeCell ref="D34:F34"/>
-    <mergeCell ref="D35:F35"/>
-    <mergeCell ref="D36:F36"/>
-    <mergeCell ref="D37:F37"/>
-    <mergeCell ref="D38:F38"/>
-    <mergeCell ref="D29:F29"/>
-    <mergeCell ref="D30:F30"/>
-    <mergeCell ref="D31:F31"/>
-    <mergeCell ref="D32:F32"/>
-    <mergeCell ref="D33:F33"/>
+  <mergeCells count="64">
+    <mergeCell ref="D56:F56"/>
+    <mergeCell ref="D57:F57"/>
+    <mergeCell ref="D58:F58"/>
+    <mergeCell ref="D59:F59"/>
+    <mergeCell ref="D51:F51"/>
+    <mergeCell ref="D52:F52"/>
+    <mergeCell ref="D53:F53"/>
+    <mergeCell ref="D54:F54"/>
+    <mergeCell ref="D55:F55"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="D48:F48"/>
+    <mergeCell ref="D49:F49"/>
+    <mergeCell ref="A50:C50"/>
+    <mergeCell ref="D25:F25"/>
+    <mergeCell ref="D26:F26"/>
+    <mergeCell ref="B1:D2"/>
+    <mergeCell ref="A8:D8"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="A12:J12"/>
+    <mergeCell ref="H5:J5"/>
+    <mergeCell ref="H6:J6"/>
+    <mergeCell ref="H7:J7"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="H4:J4"/>
+    <mergeCell ref="J9:J10"/>
+    <mergeCell ref="H3:J3"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="H9:H10"/>
+    <mergeCell ref="A11:J11"/>
     <mergeCell ref="D19:F19"/>
     <mergeCell ref="D21:F21"/>
     <mergeCell ref="D16:F16"/>
@@ -3285,24 +3618,24 @@
     <mergeCell ref="D22:F22"/>
     <mergeCell ref="D23:F23"/>
     <mergeCell ref="D24:F24"/>
-    <mergeCell ref="D25:F25"/>
-    <mergeCell ref="D26:F26"/>
-    <mergeCell ref="B1:D2"/>
-    <mergeCell ref="A8:D8"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="A12:J12"/>
-    <mergeCell ref="H5:J5"/>
-    <mergeCell ref="H6:J6"/>
-    <mergeCell ref="H7:J7"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="H4:J4"/>
-    <mergeCell ref="J9:J10"/>
-    <mergeCell ref="H3:J3"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="H9:H10"/>
-    <mergeCell ref="A11:J11"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="D29:F29"/>
+    <mergeCell ref="D30:F30"/>
+    <mergeCell ref="D31:F31"/>
+    <mergeCell ref="D32:F32"/>
+    <mergeCell ref="D33:F33"/>
+    <mergeCell ref="D34:F34"/>
+    <mergeCell ref="D35:F35"/>
+    <mergeCell ref="D36:F36"/>
+    <mergeCell ref="D37:F37"/>
+    <mergeCell ref="D38:F38"/>
+    <mergeCell ref="D44:F44"/>
+    <mergeCell ref="D45:F45"/>
+    <mergeCell ref="D46:F46"/>
+    <mergeCell ref="D39:F39"/>
+    <mergeCell ref="D40:F40"/>
+    <mergeCell ref="D41:F41"/>
+    <mergeCell ref="D42:F42"/>
+    <mergeCell ref="A43:J43"/>
   </mergeCells>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3312,20 +3645,20 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2"/>
   <cols>
-    <col min="3" max="3" width="22.75" customWidth="1"/>
-    <col min="7" max="7" width="18.75" customWidth="1"/>
+    <col min="3" max="3" width="22.77734375" customWidth="1"/>
+    <col min="7" max="7" width="18.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="22.5">
+    <row r="1" spans="1:7" ht="22.2">
       <c r="A1" s="15" t="s">
         <v>9</v>
       </c>
@@ -3345,7 +3678,7 @@
       <c r="F2" s="17"/>
       <c r="G2" s="18"/>
     </row>
-    <row r="3" spans="1:7" ht="14.25">
+    <row r="3" spans="1:7" ht="13.8">
       <c r="B3" s="19" t="s">
         <v>8</v>
       </c>
@@ -3355,7 +3688,7 @@
       <c r="F3" s="17"/>
       <c r="G3" s="18"/>
     </row>
-    <row r="4" spans="1:7" ht="14.25">
+    <row r="4" spans="1:7" ht="13.8">
       <c r="B4" s="19" t="s">
         <v>2</v>
       </c>
@@ -3365,7 +3698,7 @@
       <c r="F4" s="19"/>
       <c r="G4" s="19"/>
     </row>
-    <row r="5" spans="1:7" ht="14.25">
+    <row r="5" spans="1:7" ht="13.8">
       <c r="A5" s="19"/>
       <c r="B5" s="19"/>
       <c r="C5" s="19"/>
@@ -3374,7 +3707,7 @@
       <c r="F5" s="19"/>
       <c r="G5" s="19"/>
     </row>
-    <row r="6" spans="1:7" ht="14.25">
+    <row r="6" spans="1:7" ht="13.8">
       <c r="A6" s="19"/>
       <c r="B6" s="19"/>
       <c r="C6" s="19"/>
@@ -3383,7 +3716,7 @@
       <c r="F6" s="19"/>
       <c r="G6" s="19"/>
     </row>
-    <row r="7" spans="1:7" ht="25.5">
+    <row r="7" spans="1:7" ht="26.4">
       <c r="A7" s="20"/>
       <c r="B7" s="55" t="s">
         <v>16</v>
@@ -3404,7 +3737,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:7" s="67" customFormat="1" ht="14.25">
+    <row r="8" spans="1:7" s="67" customFormat="1" ht="13.8">
       <c r="A8" s="73"/>
       <c r="B8" s="74">
         <v>1</v>
@@ -3430,7 +3763,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="14.25">
+    <row r="9" spans="1:7" ht="13.8">
       <c r="A9" s="19"/>
       <c r="B9" s="34"/>
       <c r="C9" s="33"/>
@@ -3439,7 +3772,7 @@
       <c r="F9" s="32"/>
       <c r="G9" s="35"/>
     </row>
-    <row r="10" spans="1:7" ht="14.25">
+    <row r="10" spans="1:7" ht="13.8">
       <c r="A10" s="19"/>
       <c r="B10" s="59"/>
       <c r="C10" s="60" t="s">
@@ -3462,7 +3795,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="14.25">
+    <row r="11" spans="1:7" ht="13.8">
       <c r="A11" s="19"/>
       <c r="B11" s="21"/>
       <c r="C11" s="19"/>
@@ -3471,7 +3804,7 @@
       <c r="F11" s="23"/>
       <c r="G11" s="23"/>
     </row>
-    <row r="12" spans="1:7" ht="14.25">
+    <row r="12" spans="1:7" ht="13.8">
       <c r="A12" s="19"/>
       <c r="B12" s="19"/>
       <c r="C12" s="19" t="s">
@@ -3487,7 +3820,7 @@
       </c>
       <c r="G12" s="25"/>
     </row>
-    <row r="13" spans="1:7" ht="14.25">
+    <row r="13" spans="1:7" ht="13.8">
       <c r="A13" s="19"/>
       <c r="B13" s="19"/>
       <c r="C13" s="19" t="s">

</xml_diff>